<commit_message>
Update RRT and EST scripts, add figures, and update results
Reduced the maximum allowed runtime from 60s to 30s in both Kinematic_RRT.py and kinematic_EST.py. Updated map, start/goal, and obstacle configurations in both scripts for different test scenarios. Added new figure assets to Figures_report. Updated results Excel files for both RRT and EST experiments to reflect new runs and configurations.
</commit_message>
<xml_diff>
--- a/final project/results_kinematic_EST/map1_resultsEST.xlsx
+++ b/final project/results_kinematic_EST/map1_resultsEST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\ELEC-844\final project\results_kinematic_EST\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3522A33C-5A80-4C34-A69E-8DE421130080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44588969-7D87-4193-8812-2295E7F9074A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="7440" windowWidth="15410" windowHeight="11190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5940" yWindow="7270" windowWidth="15410" windowHeight="11190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -412,7 +412,7 @@
   <dimension ref="A1:H501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B402" sqref="B402:D501"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -452,18 +452,18 @@
         <v>4420</v>
       </c>
       <c r="C2">
-        <v>3.1819579601287842</v>
+        <v>2.767275333404541</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="F2">
         <f>AVERAGE(D2:D501)</f>
-        <v>0.97399999999999998</v>
+        <v>0.97799999999999998</v>
       </c>
       <c r="G2">
         <f>MEDIAN(C2:C501)</f>
-        <v>4.3661961555480957</v>
+        <v>3.4149365425109863</v>
       </c>
       <c r="H2">
         <f>MEDIAN(B2:B501)</f>
@@ -478,7 +478,7 @@
         <v>3027</v>
       </c>
       <c r="C3">
-        <v>2.2770102024078369</v>
+        <v>1.6241321563720701</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -492,7 +492,7 @@
         <v>11046</v>
       </c>
       <c r="C4">
-        <v>14.85342597961426</v>
+        <v>12.73072671890259</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -506,7 +506,7 @@
         <v>3088</v>
       </c>
       <c r="C5">
-        <v>1.975459098815918</v>
+        <v>1.765993118286133</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -520,7 +520,7 @@
         <v>122</v>
       </c>
       <c r="C6">
-        <v>4.9391508102416992E-2</v>
+        <v>5.0118923187255859E-2</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -534,7 +534,7 @@
         <v>9659</v>
       </c>
       <c r="C7">
-        <v>12.82926297187805</v>
+        <v>11.122737884521481</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -548,7 +548,7 @@
         <v>3426</v>
       </c>
       <c r="C8">
-        <v>2.653429508209229</v>
+        <v>2.2914965152740479</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -562,7 +562,7 @@
         <v>11418</v>
       </c>
       <c r="C9">
-        <v>18.02784967422485</v>
+        <v>14.83373045921326</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -576,7 +576,7 @@
         <v>6575</v>
       </c>
       <c r="C10">
-        <v>7.4975881576538086</v>
+        <v>6.1923074722290039</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -590,7 +590,7 @@
         <v>4727</v>
       </c>
       <c r="C11">
-        <v>4.7613012790679932</v>
+        <v>4.1420145034790039</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -604,7 +604,7 @@
         <v>1362</v>
       </c>
       <c r="C12">
-        <v>0.81297516822814941</v>
+        <v>0.75089764595031738</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -618,7 +618,7 @@
         <v>1928</v>
       </c>
       <c r="C13">
-        <v>1.25091552734375</v>
+        <v>1.178695440292358</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -632,7 +632,7 @@
         <v>3210</v>
       </c>
       <c r="C14">
-        <v>1.6073083877563481</v>
+        <v>1.5273861885070801</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -646,7 +646,7 @@
         <v>2621</v>
       </c>
       <c r="C15">
-        <v>1.563546419143677</v>
+        <v>1.427172899246216</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -660,7 +660,7 @@
         <v>6833</v>
       </c>
       <c r="C16">
-        <v>7.2475690841674796</v>
+        <v>6.6560404300689697</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -674,7 +674,7 @@
         <v>11951</v>
       </c>
       <c r="C17">
-        <v>17.602233171463009</v>
+        <v>15.511124610900881</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -688,7 +688,7 @@
         <v>4889</v>
       </c>
       <c r="C18">
-        <v>4.1801130771636963</v>
+        <v>3.6994025707244869</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -702,7 +702,7 @@
         <v>10767</v>
       </c>
       <c r="C19">
-        <v>16.358189344406131</v>
+        <v>15.81407856941223</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -716,7 +716,7 @@
         <v>13763</v>
       </c>
       <c r="C20">
-        <v>26.072539567947391</v>
+        <v>21.336426973342899</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -730,7 +730,7 @@
         <v>4023</v>
       </c>
       <c r="C21">
-        <v>3.6442091464996338</v>
+        <v>2.7787210941314702</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -744,7 +744,7 @@
         <v>8586</v>
       </c>
       <c r="C22">
-        <v>11.83730316162109</v>
+        <v>8.9079627990722656</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -758,7 +758,7 @@
         <v>1815</v>
       </c>
       <c r="C23">
-        <v>1.4071991443634031</v>
+        <v>1.0264415740966799</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -772,7 +772,7 @@
         <v>16000</v>
       </c>
       <c r="C24">
-        <v>36.423654079437263</v>
+        <v>28.413914442062381</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -783,10 +783,10 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>21571</v>
+        <v>25507</v>
       </c>
       <c r="C25">
-        <v>60.00282621383667</v>
+        <v>60.002782106399543</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -800,7 +800,7 @@
         <v>4393</v>
       </c>
       <c r="C26">
-        <v>4.0067269802093506</v>
+        <v>2.8846650123596191</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -814,7 +814,7 @@
         <v>3584</v>
       </c>
       <c r="C27">
-        <v>2.917423009872437</v>
+        <v>2.055037260055542</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -828,7 +828,7 @@
         <v>21118</v>
       </c>
       <c r="C28">
-        <v>59.192558765411377</v>
+        <v>40.361642122268677</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -842,7 +842,7 @@
         <v>3183</v>
       </c>
       <c r="C29">
-        <v>2.6036007404327388</v>
+        <v>1.6702778339385991</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -856,7 +856,7 @@
         <v>6493</v>
       </c>
       <c r="C30">
-        <v>6.9859817028045654</v>
+        <v>4.666834831237793</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -870,7 +870,7 @@
         <v>7765</v>
       </c>
       <c r="C31">
-        <v>9.1603405475616455</v>
+        <v>6.4014816284179688</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -884,7 +884,7 @@
         <v>3200</v>
       </c>
       <c r="C32">
-        <v>2.4691009521484379</v>
+        <v>1.8067131042480471</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -898,7 +898,7 @@
         <v>11730</v>
       </c>
       <c r="C33">
-        <v>18.753223657608029</v>
+        <v>13.104762554168699</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -912,7 +912,7 @@
         <v>2491</v>
       </c>
       <c r="C34">
-        <v>1.8716950416564939</v>
+        <v>1.2940788269042971</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -926,7 +926,7 @@
         <v>15405</v>
       </c>
       <c r="C35">
-        <v>32.585710287094123</v>
+        <v>24.749960660934448</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -940,7 +940,7 @@
         <v>1901</v>
       </c>
       <c r="C36">
-        <v>1.179654598236084</v>
+        <v>0.84010887145996094</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -954,7 +954,7 @@
         <v>14090</v>
       </c>
       <c r="C37">
-        <v>27.079115152359009</v>
+        <v>19.17671704292297</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -968,7 +968,7 @@
         <v>5426</v>
       </c>
       <c r="C38">
-        <v>5.1813144683837891</v>
+        <v>4.1246819496154794</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -982,7 +982,7 @@
         <v>7105</v>
       </c>
       <c r="C39">
-        <v>7.9601378440856934</v>
+        <v>5.8876736164093018</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -996,7 +996,7 @@
         <v>9311</v>
       </c>
       <c r="C40">
-        <v>13.560045957565309</v>
+        <v>10.536301374435419</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -1010,7 +1010,7 @@
         <v>787</v>
       </c>
       <c r="C41">
-        <v>0.52575063705444336</v>
+        <v>0.29933595657348627</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -1024,7 +1024,7 @@
         <v>5798</v>
       </c>
       <c r="C42">
-        <v>5.7279908657073966</v>
+        <v>4.1664776802062988</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -1038,7 +1038,7 @@
         <v>16174</v>
       </c>
       <c r="C43">
-        <v>34.65688943862915</v>
+        <v>28.6018385887146</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -1052,7 +1052,7 @@
         <v>10587</v>
       </c>
       <c r="C44">
-        <v>15.090965032577509</v>
+        <v>12.39374470710754</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -1066,7 +1066,7 @@
         <v>3404</v>
       </c>
       <c r="C45">
-        <v>3.0035297870635991</v>
+        <v>2.1722795963287349</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -1080,7 +1080,7 @@
         <v>2469</v>
       </c>
       <c r="C46">
-        <v>1.5815191268920901</v>
+        <v>1.071197509765625</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -1094,7 +1094,7 @@
         <v>10953</v>
       </c>
       <c r="C47">
-        <v>16.77236723899841</v>
+        <v>12.216629505157471</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -1108,7 +1108,7 @@
         <v>4264</v>
       </c>
       <c r="C48">
-        <v>3.6978967189788818</v>
+        <v>2.9979262351989751</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -1122,7 +1122,7 @@
         <v>7987</v>
       </c>
       <c r="C49">
-        <v>9.9522380828857422</v>
+        <v>8.4352490901947021</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -1136,7 +1136,7 @@
         <v>8553</v>
       </c>
       <c r="C50">
-        <v>10.540122747421259</v>
+        <v>8.5557818412780762</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -1150,7 +1150,7 @@
         <v>1150</v>
       </c>
       <c r="C51">
-        <v>0.68137764930725098</v>
+        <v>0.50583672523498535</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -1164,7 +1164,7 @@
         <v>1718</v>
       </c>
       <c r="C52">
-        <v>1.1348762512207029</v>
+        <v>0.81100201606750488</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -1178,7 +1178,7 @@
         <v>20764</v>
       </c>
       <c r="C53">
-        <v>56.159563302993767</v>
+        <v>44.520812034606926</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -1192,7 +1192,7 @@
         <v>9624</v>
       </c>
       <c r="C54">
-        <v>13.50861430168152</v>
+        <v>10.74039626121521</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -1206,7 +1206,7 @@
         <v>2209</v>
       </c>
       <c r="C55">
-        <v>1.315597772598267</v>
+        <v>0.98808765411376953</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -1220,7 +1220,7 @@
         <v>6919</v>
       </c>
       <c r="C56">
-        <v>7.7657818794250488</v>
+        <v>5.808436393737793</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -1234,7 +1234,7 @@
         <v>1646</v>
       </c>
       <c r="C57">
-        <v>1.0758292675018311</v>
+        <v>0.79981255531311035</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -1248,7 +1248,7 @@
         <v>1441</v>
       </c>
       <c r="C58">
-        <v>0.94313931465148926</v>
+        <v>0.61272048950195313</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -1262,7 +1262,7 @@
         <v>2388</v>
       </c>
       <c r="C59">
-        <v>1.442463636398315</v>
+        <v>1.172754287719727</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -1276,7 +1276,7 @@
         <v>5613</v>
       </c>
       <c r="C60">
-        <v>4.3320529460906982</v>
+        <v>3.4707963466644292</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -1290,7 +1290,7 @@
         <v>21590</v>
       </c>
       <c r="C61">
-        <v>54.150496006011963</v>
+        <v>43.870550155639648</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -1304,7 +1304,7 @@
         <v>10808</v>
       </c>
       <c r="C62">
-        <v>14.473387241363531</v>
+        <v>12.960101366043091</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -1318,7 +1318,7 @@
         <v>3368</v>
       </c>
       <c r="C63">
-        <v>2.049186229705811</v>
+        <v>1.7032203674316411</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -1332,7 +1332,7 @@
         <v>849</v>
       </c>
       <c r="C64">
-        <v>0.40875101089477539</v>
+        <v>0.37639808654785162</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -1346,7 +1346,7 @@
         <v>3015</v>
       </c>
       <c r="C65">
-        <v>1.918433666229248</v>
+        <v>1.7543585300445561</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -1360,7 +1360,7 @@
         <v>7089</v>
       </c>
       <c r="C66">
-        <v>7.6248447895050049</v>
+        <v>6.6419787406921387</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -1374,7 +1374,7 @@
         <v>8476</v>
       </c>
       <c r="C67">
-        <v>9.2371683120727539</v>
+        <v>9.0467913150787354</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -1388,7 +1388,7 @@
         <v>8530</v>
       </c>
       <c r="C68">
-        <v>9.7941319942474365</v>
+        <v>7.9687521457672119</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -1402,7 +1402,7 @@
         <v>6029</v>
       </c>
       <c r="C69">
-        <v>5.3207776546478271</v>
+        <v>4.7615346908569336</v>
       </c>
       <c r="D69">
         <v>1</v>
@@ -1416,7 +1416,7 @@
         <v>2194</v>
       </c>
       <c r="C70">
-        <v>0.8148796558380127</v>
+        <v>0.6672215461730957</v>
       </c>
       <c r="D70">
         <v>1</v>
@@ -1430,7 +1430,7 @@
         <v>10483</v>
       </c>
       <c r="C71">
-        <v>10.250389337539669</v>
+        <v>8.4222464561462402</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -1444,7 +1444,7 @@
         <v>2198</v>
       </c>
       <c r="C72">
-        <v>1.272723436355591</v>
+        <v>1.099310636520386</v>
       </c>
       <c r="D72">
         <v>1</v>
@@ -1458,7 +1458,7 @@
         <v>2304</v>
       </c>
       <c r="C73">
-        <v>1.101078987121582</v>
+        <v>0.85633993148803711</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -1472,7 +1472,7 @@
         <v>4371</v>
       </c>
       <c r="C74">
-        <v>3.4545795917510991</v>
+        <v>2.850404024124146</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -1486,7 +1486,7 @@
         <v>9433</v>
       </c>
       <c r="C75">
-        <v>12.13186836242676</v>
+        <v>10.06337308883667</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -1500,7 +1500,7 @@
         <v>6886</v>
       </c>
       <c r="C76">
-        <v>7.3205397129058838</v>
+        <v>5.7586767673492432</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -1514,7 +1514,7 @@
         <v>9631</v>
       </c>
       <c r="C77">
-        <v>9.7868125438690186</v>
+        <v>8.9811844825744629</v>
       </c>
       <c r="D77">
         <v>1</v>
@@ -1528,7 +1528,7 @@
         <v>9986</v>
       </c>
       <c r="C78">
-        <v>11.81279826164246</v>
+        <v>10.872476577758791</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -1542,7 +1542,7 @@
         <v>1861</v>
       </c>
       <c r="C79">
-        <v>0.9771730899810791</v>
+        <v>0.86034202575683594</v>
       </c>
       <c r="D79">
         <v>1</v>
@@ -1556,7 +1556,7 @@
         <v>3642</v>
       </c>
       <c r="C80">
-        <v>2.5463485717773442</v>
+        <v>2.224096298217773</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -1570,7 +1570,7 @@
         <v>4908</v>
       </c>
       <c r="C81">
-        <v>3.7640914916992192</v>
+        <v>3.3578529357910161</v>
       </c>
       <c r="D81">
         <v>1</v>
@@ -1584,7 +1584,7 @@
         <v>13979</v>
       </c>
       <c r="C82">
-        <v>19.646795511245731</v>
+        <v>17.207143068313599</v>
       </c>
       <c r="D82">
         <v>1</v>
@@ -1598,7 +1598,7 @@
         <v>4865</v>
       </c>
       <c r="C83">
-        <v>3.4968760013580318</v>
+        <v>3.2598872184753418</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -1612,7 +1612,7 @@
         <v>1923</v>
       </c>
       <c r="C84">
-        <v>1.044136524200439</v>
+        <v>0.9256594181060791</v>
       </c>
       <c r="D84">
         <v>1</v>
@@ -1626,7 +1626,7 @@
         <v>5418</v>
       </c>
       <c r="C85">
-        <v>4.4614808559417716</v>
+        <v>3.9776806831359859</v>
       </c>
       <c r="D85">
         <v>1</v>
@@ -1640,7 +1640,7 @@
         <v>1822</v>
       </c>
       <c r="C86">
-        <v>0.9581606388092041</v>
+        <v>0.81700634956359863</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -1654,7 +1654,7 @@
         <v>16770</v>
       </c>
       <c r="C87">
-        <v>28.865922212600712</v>
+        <v>25.4084038734436</v>
       </c>
       <c r="D87">
         <v>1</v>
@@ -1668,7 +1668,7 @@
         <v>2454</v>
       </c>
       <c r="C88">
-        <v>1.159313440322876</v>
+        <v>1.091157913208008</v>
       </c>
       <c r="D88">
         <v>1</v>
@@ -1682,7 +1682,7 @@
         <v>12218</v>
       </c>
       <c r="C89">
-        <v>16.448955535888668</v>
+        <v>14.843362808227541</v>
       </c>
       <c r="D89">
         <v>1</v>
@@ -1696,7 +1696,7 @@
         <v>8483</v>
       </c>
       <c r="C90">
-        <v>8.0746560096740723</v>
+        <v>7.8247604370117188</v>
       </c>
       <c r="D90">
         <v>1</v>
@@ -1710,7 +1710,7 @@
         <v>7254</v>
       </c>
       <c r="C91">
-        <v>7.0101156234741211</v>
+        <v>6.4837729930877694</v>
       </c>
       <c r="D91">
         <v>1</v>
@@ -1724,7 +1724,7 @@
         <v>14943</v>
       </c>
       <c r="C92">
-        <v>22.595946788787838</v>
+        <v>20.924720525741581</v>
       </c>
       <c r="D92">
         <v>1</v>
@@ -1738,7 +1738,7 @@
         <v>1851</v>
       </c>
       <c r="C93">
-        <v>1.184374094009399</v>
+        <v>0.80437660217285156</v>
       </c>
       <c r="D93">
         <v>1</v>
@@ -1752,7 +1752,7 @@
         <v>8277</v>
       </c>
       <c r="C94">
-        <v>8.5980219841003418</v>
+        <v>7.7488558292388916</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -1766,7 +1766,7 @@
         <v>4441</v>
       </c>
       <c r="C95">
-        <v>2.7638499736785889</v>
+        <v>2.8772623538970952</v>
       </c>
       <c r="D95">
         <v>1</v>
@@ -1780,7 +1780,7 @@
         <v>3901</v>
       </c>
       <c r="C96">
-        <v>2.2798244953155522</v>
+        <v>2.4300322532653809</v>
       </c>
       <c r="D96">
         <v>1</v>
@@ -1794,7 +1794,7 @@
         <v>1884</v>
       </c>
       <c r="C97">
-        <v>0.81582164764404297</v>
+        <v>0.88064455986022949</v>
       </c>
       <c r="D97">
         <v>1</v>
@@ -1808,7 +1808,7 @@
         <v>2565</v>
       </c>
       <c r="C98">
-        <v>1.364470958709717</v>
+        <v>1.303118944168091</v>
       </c>
       <c r="D98">
         <v>1</v>
@@ -1822,7 +1822,7 @@
         <v>1558</v>
       </c>
       <c r="C99">
-        <v>0.58040261268615723</v>
+        <v>0.60640311241149902</v>
       </c>
       <c r="D99">
         <v>1</v>
@@ -1836,7 +1836,7 @@
         <v>9021</v>
       </c>
       <c r="C100">
-        <v>7.6826198101043701</v>
+        <v>7.5163688659667969</v>
       </c>
       <c r="D100">
         <v>1</v>
@@ -1850,7 +1850,7 @@
         <v>134</v>
       </c>
       <c r="C101">
-        <v>4.0230989456176758E-2</v>
+        <v>3.9577484130859382E-2</v>
       </c>
       <c r="D101">
         <v>1</v>
@@ -1864,7 +1864,7 @@
         <v>10886</v>
       </c>
       <c r="C102">
-        <v>14.66747212409973</v>
+        <v>12.693410873413089</v>
       </c>
       <c r="D102">
         <v>1</v>
@@ -1878,7 +1878,7 @@
         <v>4741</v>
       </c>
       <c r="C103">
-        <v>2.3160421848297119</v>
+        <v>2.1474189758300781</v>
       </c>
       <c r="D103">
         <v>1</v>
@@ -1892,7 +1892,7 @@
         <v>5075</v>
       </c>
       <c r="C104">
-        <v>3.4559330940246582</v>
+        <v>3.1379368305206299</v>
       </c>
       <c r="D104">
         <v>1</v>
@@ -1906,7 +1906,7 @@
         <v>12309</v>
       </c>
       <c r="C105">
-        <v>18.565956592559811</v>
+        <v>15.35720777511597</v>
       </c>
       <c r="D105">
         <v>1</v>
@@ -1920,7 +1920,7 @@
         <v>8695</v>
       </c>
       <c r="C106">
-        <v>12.029433488845831</v>
+        <v>9.8235311508178711</v>
       </c>
       <c r="D106">
         <v>1</v>
@@ -1934,7 +1934,7 @@
         <v>6545</v>
       </c>
       <c r="C107">
-        <v>7.9987812042236328</v>
+        <v>6.8526706695556641</v>
       </c>
       <c r="D107">
         <v>1</v>
@@ -1948,7 +1948,7 @@
         <v>2781</v>
       </c>
       <c r="C108">
-        <v>2.1940042972564702</v>
+        <v>1.830486059188843</v>
       </c>
       <c r="D108">
         <v>1</v>
@@ -1962,7 +1962,7 @@
         <v>4635</v>
       </c>
       <c r="C109">
-        <v>4.1115553379058838</v>
+        <v>3.624930620193481</v>
       </c>
       <c r="D109">
         <v>1</v>
@@ -1976,7 +1976,7 @@
         <v>10072</v>
       </c>
       <c r="C110">
-        <v>15.5935001373291</v>
+        <v>13.06898617744446</v>
       </c>
       <c r="D110">
         <v>1</v>
@@ -1990,7 +1990,7 @@
         <v>10213</v>
       </c>
       <c r="C111">
-        <v>15.313825368881229</v>
+        <v>13.95496845245361</v>
       </c>
       <c r="D111">
         <v>1</v>
@@ -2001,10 +2001,10 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>20118</v>
+        <v>23397</v>
       </c>
       <c r="C112">
-        <v>60.004831075668328</v>
+        <v>60.002418756484992</v>
       </c>
       <c r="D112">
         <v>0</v>
@@ -2018,7 +2018,7 @@
         <v>6675</v>
       </c>
       <c r="C113">
-        <v>8.1654915809631348</v>
+        <v>5.6965217590332031</v>
       </c>
       <c r="D113">
         <v>1</v>
@@ -2032,7 +2032,7 @@
         <v>11804</v>
       </c>
       <c r="C114">
-        <v>18.596822738647461</v>
+        <v>13.743661403656009</v>
       </c>
       <c r="D114">
         <v>1</v>
@@ -2046,7 +2046,7 @@
         <v>3195</v>
       </c>
       <c r="C115">
-        <v>2.4177989959716801</v>
+        <v>1.783372640609741</v>
       </c>
       <c r="D115">
         <v>1</v>
@@ -2060,7 +2060,7 @@
         <v>3905</v>
       </c>
       <c r="C116">
-        <v>3.3963406085968022</v>
+        <v>2.366245031356812</v>
       </c>
       <c r="D116">
         <v>1</v>
@@ -2074,7 +2074,7 @@
         <v>8602</v>
       </c>
       <c r="C117">
-        <v>11.56045341491699</v>
+        <v>8.0007145404815674</v>
       </c>
       <c r="D117">
         <v>1</v>
@@ -2088,7 +2088,7 @@
         <v>14408</v>
       </c>
       <c r="C118">
-        <v>28.63689208030701</v>
+        <v>20.446263790130619</v>
       </c>
       <c r="D118">
         <v>1</v>
@@ -2102,7 +2102,7 @@
         <v>12037</v>
       </c>
       <c r="C119">
-        <v>21.079772472381588</v>
+        <v>14.958354711532589</v>
       </c>
       <c r="D119">
         <v>1</v>
@@ -2116,7 +2116,7 @@
         <v>3504</v>
       </c>
       <c r="C120">
-        <v>2.7819914817810059</v>
+        <v>1.9997601509094241</v>
       </c>
       <c r="D120">
         <v>1</v>
@@ -2130,7 +2130,7 @@
         <v>745</v>
       </c>
       <c r="C121">
-        <v>0.34914422035217291</v>
+        <v>0.25824522972106928</v>
       </c>
       <c r="D121">
         <v>1</v>
@@ -2144,7 +2144,7 @@
         <v>3727</v>
       </c>
       <c r="C122">
-        <v>2.7143301963806148</v>
+        <v>1.7460823059082029</v>
       </c>
       <c r="D122">
         <v>1</v>
@@ -2155,10 +2155,10 @@
         <v>121</v>
       </c>
       <c r="B123">
-        <v>21678</v>
+        <v>26106</v>
       </c>
       <c r="C123">
-        <v>60.001470327377319</v>
+        <v>60.005009174346917</v>
       </c>
       <c r="D123">
         <v>0</v>
@@ -2172,7 +2172,7 @@
         <v>10517</v>
       </c>
       <c r="C124">
-        <v>17.563923597335819</v>
+        <v>11.653135299682621</v>
       </c>
       <c r="D124">
         <v>1</v>
@@ -2183,10 +2183,10 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>21114</v>
+        <v>25214</v>
       </c>
       <c r="C125">
-        <v>60.004081964492798</v>
+        <v>60.002902746200562</v>
       </c>
       <c r="D125">
         <v>0</v>
@@ -2200,7 +2200,7 @@
         <v>4303</v>
       </c>
       <c r="C126">
-        <v>3.755912303924561</v>
+        <v>3.0076115131378169</v>
       </c>
       <c r="D126">
         <v>1</v>
@@ -2214,7 +2214,7 @@
         <v>1262</v>
       </c>
       <c r="C127">
-        <v>0.6660773754119873</v>
+        <v>0.56374454498291016</v>
       </c>
       <c r="D127">
         <v>1</v>
@@ -2228,7 +2228,7 @@
         <v>5866</v>
       </c>
       <c r="C128">
-        <v>5.987668514251709</v>
+        <v>4.0287604331970206</v>
       </c>
       <c r="D128">
         <v>1</v>
@@ -2242,7 +2242,7 @@
         <v>3629</v>
       </c>
       <c r="C129">
-        <v>3.1833546161651611</v>
+        <v>2.1666867733001709</v>
       </c>
       <c r="D129">
         <v>1</v>
@@ -2256,7 +2256,7 @@
         <v>3641</v>
       </c>
       <c r="C130">
-        <v>3.1849231719970699</v>
+        <v>2.2273504734039311</v>
       </c>
       <c r="D130">
         <v>1</v>
@@ -2270,7 +2270,7 @@
         <v>9169</v>
       </c>
       <c r="C131">
-        <v>12.78703737258911</v>
+        <v>10.29142379760742</v>
       </c>
       <c r="D131">
         <v>1</v>
@@ -2284,7 +2284,7 @@
         <v>2288</v>
       </c>
       <c r="C132">
-        <v>0.83644866943359375</v>
+        <v>0.73677873611450195</v>
       </c>
       <c r="D132">
         <v>1</v>
@@ -2298,7 +2298,7 @@
         <v>7838</v>
       </c>
       <c r="C133">
-        <v>8.7719066143035889</v>
+        <v>6.2691497802734384</v>
       </c>
       <c r="D133">
         <v>1</v>
@@ -2312,7 +2312,7 @@
         <v>1147</v>
       </c>
       <c r="C134">
-        <v>0.53934192657470703</v>
+        <v>0.38288736343383789</v>
       </c>
       <c r="D134">
         <v>1</v>
@@ -2326,7 +2326,7 @@
         <v>2492</v>
       </c>
       <c r="C135">
-        <v>1.9280505180358889</v>
+        <v>1.721743106842041</v>
       </c>
       <c r="D135">
         <v>1</v>
@@ -2340,7 +2340,7 @@
         <v>14912</v>
       </c>
       <c r="C136">
-        <v>30.989757299423221</v>
+        <v>25.423849821090698</v>
       </c>
       <c r="D136">
         <v>1</v>
@@ -2354,7 +2354,7 @@
         <v>1029</v>
       </c>
       <c r="C137">
-        <v>0.64591670036315918</v>
+        <v>0.39627623558044428</v>
       </c>
       <c r="D137">
         <v>1</v>
@@ -2368,7 +2368,7 @@
         <v>12974</v>
       </c>
       <c r="C138">
-        <v>22.835998773574829</v>
+        <v>17.48500752449036</v>
       </c>
       <c r="D138">
         <v>1</v>
@@ -2379,10 +2379,10 @@
         <v>137</v>
       </c>
       <c r="B139">
-        <v>21805</v>
+        <v>25555</v>
       </c>
       <c r="C139">
-        <v>60.00261926651001</v>
+        <v>60.001325368881233</v>
       </c>
       <c r="D139">
         <v>0</v>
@@ -2396,7 +2396,7 @@
         <v>5826</v>
       </c>
       <c r="C140">
-        <v>6.3765852451324463</v>
+        <v>4.7751839160919189</v>
       </c>
       <c r="D140">
         <v>1</v>
@@ -2410,7 +2410,7 @@
         <v>3509</v>
       </c>
       <c r="C141">
-        <v>2.8271503448486328</v>
+        <v>1.973501443862915</v>
       </c>
       <c r="D141">
         <v>1</v>
@@ -2424,7 +2424,7 @@
         <v>4051</v>
       </c>
       <c r="C142">
-        <v>3.5596330165863042</v>
+        <v>2.4343748092651372</v>
       </c>
       <c r="D142">
         <v>1</v>
@@ -2438,7 +2438,7 @@
         <v>2236</v>
       </c>
       <c r="C143">
-        <v>1.443057060241699</v>
+        <v>0.98772263526916504</v>
       </c>
       <c r="D143">
         <v>1</v>
@@ -2452,7 +2452,7 @@
         <v>8963</v>
       </c>
       <c r="C144">
-        <v>12.0093150138855</v>
+        <v>8.6116888523101807</v>
       </c>
       <c r="D144">
         <v>1</v>
@@ -2466,7 +2466,7 @@
         <v>5651</v>
       </c>
       <c r="C145">
-        <v>5.8663852214813232</v>
+        <v>3.8192276954650879</v>
       </c>
       <c r="D145">
         <v>1</v>
@@ -2480,7 +2480,7 @@
         <v>15898</v>
       </c>
       <c r="C146">
-        <v>32.739790678024292</v>
+        <v>24.027426719665531</v>
       </c>
       <c r="D146">
         <v>1</v>
@@ -2494,7 +2494,7 @@
         <v>3440</v>
       </c>
       <c r="C147">
-        <v>2.5524494647979741</v>
+        <v>1.8930761814117429</v>
       </c>
       <c r="D147">
         <v>1</v>
@@ -2508,7 +2508,7 @@
         <v>9353</v>
       </c>
       <c r="C148">
-        <v>12.46717739105225</v>
+        <v>9.3055179119110107</v>
       </c>
       <c r="D148">
         <v>1</v>
@@ -2522,7 +2522,7 @@
         <v>16540</v>
       </c>
       <c r="C149">
-        <v>33.950778245925903</v>
+        <v>27.722307443618771</v>
       </c>
       <c r="D149">
         <v>1</v>
@@ -2536,7 +2536,7 @@
         <v>3702</v>
       </c>
       <c r="C150">
-        <v>2.7503986358642578</v>
+        <v>2.255652904510498</v>
       </c>
       <c r="D150">
         <v>1</v>
@@ -2550,7 +2550,7 @@
         <v>3764</v>
       </c>
       <c r="C151">
-        <v>2.6727206707000728</v>
+        <v>2.236135721206665</v>
       </c>
       <c r="D151">
         <v>1</v>
@@ -2564,7 +2564,7 @@
         <v>5230</v>
       </c>
       <c r="C152">
-        <v>4.4777400493621826</v>
+        <v>4.6885471343994141</v>
       </c>
       <c r="D152">
         <v>1</v>
@@ -2578,7 +2578,7 @@
         <v>6228</v>
       </c>
       <c r="C153">
-        <v>5.0571599006652832</v>
+        <v>4.7473244667053223</v>
       </c>
       <c r="D153">
         <v>1</v>
@@ -2592,7 +2592,7 @@
         <v>3491</v>
       </c>
       <c r="C154">
-        <v>2.4948828220367432</v>
+        <v>2.116340160369873</v>
       </c>
       <c r="D154">
         <v>1</v>
@@ -2606,7 +2606,7 @@
         <v>4557</v>
       </c>
       <c r="C155">
-        <v>3.713074684143066</v>
+        <v>3.3634617328643799</v>
       </c>
       <c r="D155">
         <v>1</v>
@@ -2620,7 +2620,7 @@
         <v>1393</v>
       </c>
       <c r="C156">
-        <v>0.79905986785888672</v>
+        <v>0.64867043495178223</v>
       </c>
       <c r="D156">
         <v>1</v>
@@ -2634,7 +2634,7 @@
         <v>4152</v>
       </c>
       <c r="C157">
-        <v>3.095538854598999</v>
+        <v>2.4156944751739502</v>
       </c>
       <c r="D157">
         <v>1</v>
@@ -2648,7 +2648,7 @@
         <v>2525</v>
       </c>
       <c r="C158">
-        <v>1.169862747192383</v>
+        <v>0.94958138465881348</v>
       </c>
       <c r="D158">
         <v>1</v>
@@ -2662,7 +2662,7 @@
         <v>3591</v>
       </c>
       <c r="C159">
-        <v>2.3029220104217529</v>
+        <v>1.8697319030761721</v>
       </c>
       <c r="D159">
         <v>1</v>
@@ -2676,7 +2676,7 @@
         <v>6862</v>
       </c>
       <c r="C160">
-        <v>7.07698655128479</v>
+        <v>5.9823846817016602</v>
       </c>
       <c r="D160">
         <v>1</v>
@@ -2690,7 +2690,7 @@
         <v>12851</v>
       </c>
       <c r="C161">
-        <v>11.77993416786194</v>
+        <v>9.5338447093963623</v>
       </c>
       <c r="D161">
         <v>1</v>
@@ -2704,7 +2704,7 @@
         <v>6858</v>
       </c>
       <c r="C162">
-        <v>6.2806353569030762</v>
+        <v>5.1502642631530762</v>
       </c>
       <c r="D162">
         <v>1</v>
@@ -2718,7 +2718,7 @@
         <v>1879</v>
       </c>
       <c r="C163">
-        <v>1.0944733619689939</v>
+        <v>0.95290231704711914</v>
       </c>
       <c r="D163">
         <v>1</v>
@@ -2732,7 +2732,7 @@
         <v>3588</v>
       </c>
       <c r="C164">
-        <v>2.5639240741729741</v>
+        <v>2.2240614891052251</v>
       </c>
       <c r="D164">
         <v>1</v>
@@ -2746,7 +2746,7 @@
         <v>7698</v>
       </c>
       <c r="C165">
-        <v>8.1912503242492676</v>
+        <v>7.0178298950195313</v>
       </c>
       <c r="D165">
         <v>1</v>
@@ -2760,7 +2760,7 @@
         <v>2714</v>
       </c>
       <c r="C166">
-        <v>1.6445989608764651</v>
+        <v>1.572695255279541</v>
       </c>
       <c r="D166">
         <v>1</v>
@@ -2774,7 +2774,7 @@
         <v>320</v>
       </c>
       <c r="C167">
-        <v>0.1259160041809082</v>
+        <v>0.1202051639556885</v>
       </c>
       <c r="D167">
         <v>1</v>
@@ -2788,7 +2788,7 @@
         <v>6024</v>
       </c>
       <c r="C168">
-        <v>5.1986777782440194</v>
+        <v>4.8493471145629883</v>
       </c>
       <c r="D168">
         <v>1</v>
@@ -2802,7 +2802,7 @@
         <v>4733</v>
       </c>
       <c r="C169">
-        <v>2.7469696998596191</v>
+        <v>2.0786328315734859</v>
       </c>
       <c r="D169">
         <v>1</v>
@@ -2816,7 +2816,7 @@
         <v>6217</v>
       </c>
       <c r="C170">
-        <v>5.6014742851257324</v>
+        <v>4.9385442733764648</v>
       </c>
       <c r="D170">
         <v>1</v>
@@ -2830,7 +2830,7 @@
         <v>7493</v>
       </c>
       <c r="C171">
-        <v>7.8377914428710938</v>
+        <v>6.9792928695678711</v>
       </c>
       <c r="D171">
         <v>1</v>
@@ -2844,7 +2844,7 @@
         <v>6487</v>
       </c>
       <c r="C172">
-        <v>5.913616418838501</v>
+        <v>5.2244217395782471</v>
       </c>
       <c r="D172">
         <v>1</v>
@@ -2858,7 +2858,7 @@
         <v>2473</v>
       </c>
       <c r="C173">
-        <v>1.560466051101685</v>
+        <v>1.505780935287476</v>
       </c>
       <c r="D173">
         <v>1</v>
@@ -2872,7 +2872,7 @@
         <v>1724</v>
       </c>
       <c r="C174">
-        <v>0.85546565055847168</v>
+        <v>0.76381206512451172</v>
       </c>
       <c r="D174">
         <v>1</v>
@@ -2886,7 +2886,7 @@
         <v>2998</v>
       </c>
       <c r="C175">
-        <v>1.6003150939941411</v>
+        <v>1.512568473815918</v>
       </c>
       <c r="D175">
         <v>1</v>
@@ -2900,7 +2900,7 @@
         <v>9452</v>
       </c>
       <c r="C176">
-        <v>11.619813919067379</v>
+        <v>9.790473461151123</v>
       </c>
       <c r="D176">
         <v>1</v>
@@ -2914,7 +2914,7 @@
         <v>9651</v>
       </c>
       <c r="C177">
-        <v>9.9765160083770752</v>
+        <v>8.9113767147064209</v>
       </c>
       <c r="D177">
         <v>1</v>
@@ -2928,7 +2928,7 @@
         <v>1109</v>
       </c>
       <c r="C178">
-        <v>0.50988221168518066</v>
+        <v>0.46060681343078608</v>
       </c>
       <c r="D178">
         <v>1</v>
@@ -2942,7 +2942,7 @@
         <v>7344</v>
       </c>
       <c r="C179">
-        <v>4.2909550666809082</v>
+        <v>3.806559562683105</v>
       </c>
       <c r="D179">
         <v>1</v>
@@ -2956,7 +2956,7 @@
         <v>2797</v>
       </c>
       <c r="C180">
-        <v>1.5487275123596189</v>
+        <v>1.332084178924561</v>
       </c>
       <c r="D180">
         <v>1</v>
@@ -2970,7 +2970,7 @@
         <v>10338</v>
       </c>
       <c r="C181">
-        <v>13.860697984695429</v>
+        <v>11.88009285926819</v>
       </c>
       <c r="D181">
         <v>1</v>
@@ -2984,7 +2984,7 @@
         <v>6353</v>
       </c>
       <c r="C182">
-        <v>5.6950294971466056</v>
+        <v>5.3095452785491943</v>
       </c>
       <c r="D182">
         <v>1</v>
@@ -2998,7 +2998,7 @@
         <v>8595</v>
       </c>
       <c r="C183">
-        <v>8.6292455196380615</v>
+        <v>7.0282473564147949</v>
       </c>
       <c r="D183">
         <v>1</v>
@@ -3012,7 +3012,7 @@
         <v>3112</v>
       </c>
       <c r="C184">
-        <v>1.6692550182342529</v>
+        <v>1.497905015945435</v>
       </c>
       <c r="D184">
         <v>1</v>
@@ -3026,7 +3026,7 @@
         <v>3701</v>
       </c>
       <c r="C185">
-        <v>2.5284569263458252</v>
+        <v>2.027366161346436</v>
       </c>
       <c r="D185">
         <v>1</v>
@@ -3040,7 +3040,7 @@
         <v>4531</v>
       </c>
       <c r="C186">
-        <v>3.4313488006591801</v>
+        <v>2.8226766586303711</v>
       </c>
       <c r="D186">
         <v>1</v>
@@ -3054,7 +3054,7 @@
         <v>550</v>
       </c>
       <c r="C187">
-        <v>0.21094083786010739</v>
+        <v>0.20805668830871579</v>
       </c>
       <c r="D187">
         <v>1</v>
@@ -3068,7 +3068,7 @@
         <v>9756</v>
       </c>
       <c r="C188">
-        <v>12.44311475753784</v>
+        <v>10.747797727584841</v>
       </c>
       <c r="D188">
         <v>1</v>
@@ -3082,7 +3082,7 @@
         <v>8624</v>
       </c>
       <c r="C189">
-        <v>11.068933248519899</v>
+        <v>9.024158239364624</v>
       </c>
       <c r="D189">
         <v>1</v>
@@ -3096,7 +3096,7 @@
         <v>7767</v>
       </c>
       <c r="C190">
-        <v>7.3867170810699463</v>
+        <v>6.7011368274688721</v>
       </c>
       <c r="D190">
         <v>1</v>
@@ -3110,7 +3110,7 @@
         <v>13761</v>
       </c>
       <c r="C191">
-        <v>21.19321966171265</v>
+        <v>18.510257005691528</v>
       </c>
       <c r="D191">
         <v>1</v>
@@ -3124,7 +3124,7 @@
         <v>2973</v>
       </c>
       <c r="C192">
-        <v>1.513774633407593</v>
+        <v>1.2982625961303711</v>
       </c>
       <c r="D192">
         <v>1</v>
@@ -3138,7 +3138,7 @@
         <v>3262</v>
       </c>
       <c r="C193">
-        <v>1.8328850269317629</v>
+        <v>1.7308540344238279</v>
       </c>
       <c r="D193">
         <v>1</v>
@@ -3152,7 +3152,7 @@
         <v>2561</v>
       </c>
       <c r="C194">
-        <v>1.1132709980010991</v>
+        <v>1.1060736179351811</v>
       </c>
       <c r="D194">
         <v>1</v>
@@ -3166,7 +3166,7 @@
         <v>3355</v>
       </c>
       <c r="C195">
-        <v>1.789753913879395</v>
+        <v>1.7594437599182129</v>
       </c>
       <c r="D195">
         <v>1</v>
@@ -3180,7 +3180,7 @@
         <v>6480</v>
       </c>
       <c r="C196">
-        <v>5.7393679618835449</v>
+        <v>5.0633330345153809</v>
       </c>
       <c r="D196">
         <v>1</v>
@@ -3194,7 +3194,7 @@
         <v>6394</v>
       </c>
       <c r="C197">
-        <v>5.2924537658691406</v>
+        <v>4.8122010231018066</v>
       </c>
       <c r="D197">
         <v>1</v>
@@ -3208,7 +3208,7 @@
         <v>2318</v>
       </c>
       <c r="C198">
-        <v>0.99320149421691895</v>
+        <v>0.90140008926391602</v>
       </c>
       <c r="D198">
         <v>1</v>
@@ -3222,7 +3222,7 @@
         <v>3103</v>
       </c>
       <c r="C199">
-        <v>1.908838272094727</v>
+        <v>1.606194019317627</v>
       </c>
       <c r="D199">
         <v>1</v>
@@ -3236,7 +3236,7 @@
         <v>4717</v>
       </c>
       <c r="C200">
-        <v>3.7757325172424321</v>
+        <v>2.8034884929656978</v>
       </c>
       <c r="D200">
         <v>1</v>
@@ -3250,7 +3250,7 @@
         <v>3712</v>
       </c>
       <c r="C201">
-        <v>2.323147296905518</v>
+        <v>1.956302165985107</v>
       </c>
       <c r="D201">
         <v>1</v>
@@ -3264,7 +3264,7 @@
         <v>1537</v>
       </c>
       <c r="C202">
-        <v>1.1576123237609861</v>
+        <v>0.77187061309814453</v>
       </c>
       <c r="D202">
         <v>1</v>
@@ -3278,7 +3278,7 @@
         <v>1748</v>
       </c>
       <c r="C203">
-        <v>0.97828865051269531</v>
+        <v>0.87320065498352051</v>
       </c>
       <c r="D203">
         <v>1</v>
@@ -3292,7 +3292,7 @@
         <v>2906</v>
       </c>
       <c r="C204">
-        <v>1.8734233379364009</v>
+        <v>1.6247880458831789</v>
       </c>
       <c r="D204">
         <v>1</v>
@@ -3306,7 +3306,7 @@
         <v>9435</v>
       </c>
       <c r="C205">
-        <v>11.62699031829834</v>
+        <v>9.9083728790283203</v>
       </c>
       <c r="D205">
         <v>1</v>
@@ -3320,7 +3320,7 @@
         <v>3980</v>
       </c>
       <c r="C206">
-        <v>3.46942138671875</v>
+        <v>2.881757497787476</v>
       </c>
       <c r="D206">
         <v>1</v>
@@ -3334,7 +3334,7 @@
         <v>9161</v>
       </c>
       <c r="C207">
-        <v>12.307098627090451</v>
+        <v>10.117634057998661</v>
       </c>
       <c r="D207">
         <v>1</v>
@@ -3348,7 +3348,7 @@
         <v>4384</v>
       </c>
       <c r="C208">
-        <v>3.7394957542419429</v>
+        <v>3.039589643478394</v>
       </c>
       <c r="D208">
         <v>1</v>
@@ -3362,7 +3362,7 @@
         <v>1368</v>
       </c>
       <c r="C209">
-        <v>0.92295169830322266</v>
+        <v>0.8540494441986084</v>
       </c>
       <c r="D209">
         <v>1</v>
@@ -3376,7 +3376,7 @@
         <v>2853</v>
       </c>
       <c r="C210">
-        <v>2.2121303081512451</v>
+        <v>1.8821818828582759</v>
       </c>
       <c r="D210">
         <v>1</v>
@@ -3390,7 +3390,7 @@
         <v>11676</v>
       </c>
       <c r="C211">
-        <v>19.006242990493771</v>
+        <v>15.58777832984924</v>
       </c>
       <c r="D211">
         <v>1</v>
@@ -3404,7 +3404,7 @@
         <v>3812</v>
       </c>
       <c r="C212">
-        <v>3.594968318939209</v>
+        <v>2.7155590057373051</v>
       </c>
       <c r="D212">
         <v>1</v>
@@ -3418,7 +3418,7 @@
         <v>19975</v>
       </c>
       <c r="C213">
-        <v>51.688498020172119</v>
+        <v>43.015792369842529</v>
       </c>
       <c r="D213">
         <v>1</v>
@@ -3432,7 +3432,7 @@
         <v>2474</v>
       </c>
       <c r="C214">
-        <v>1.9389364719390869</v>
+        <v>1.634118318557739</v>
       </c>
       <c r="D214">
         <v>1</v>
@@ -3446,7 +3446,7 @@
         <v>5324</v>
       </c>
       <c r="C215">
-        <v>5.4299118518829346</v>
+        <v>4.4712100028991699</v>
       </c>
       <c r="D215">
         <v>1</v>
@@ -3460,7 +3460,7 @@
         <v>5457</v>
       </c>
       <c r="C216">
-        <v>5.9432649612426758</v>
+        <v>4.4957554340362549</v>
       </c>
       <c r="D216">
         <v>1</v>
@@ -3474,7 +3474,7 @@
         <v>10629</v>
       </c>
       <c r="C217">
-        <v>16.937326192855831</v>
+        <v>13.41584444046021</v>
       </c>
       <c r="D217">
         <v>1</v>
@@ -3488,7 +3488,7 @@
         <v>2528</v>
       </c>
       <c r="C218">
-        <v>1.836154699325562</v>
+        <v>1.444885730743408</v>
       </c>
       <c r="D218">
         <v>1</v>
@@ -3502,7 +3502,7 @@
         <v>3127</v>
       </c>
       <c r="C219">
-        <v>1.6881618499755859</v>
+        <v>1.3330497741699221</v>
       </c>
       <c r="D219">
         <v>1</v>
@@ -3516,7 +3516,7 @@
         <v>3061</v>
       </c>
       <c r="C220">
-        <v>2.3474941253662109</v>
+        <v>1.8783764839172361</v>
       </c>
       <c r="D220">
         <v>1</v>
@@ -3530,7 +3530,7 @@
         <v>9802</v>
       </c>
       <c r="C221">
-        <v>13.705987691879271</v>
+        <v>10.479140520095831</v>
       </c>
       <c r="D221">
         <v>1</v>
@@ -3544,7 +3544,7 @@
         <v>11050</v>
       </c>
       <c r="C222">
-        <v>17.613716602325439</v>
+        <v>12.16622686386108</v>
       </c>
       <c r="D222">
         <v>1</v>
@@ -3558,7 +3558,7 @@
         <v>8363</v>
       </c>
       <c r="C223">
-        <v>11.096625089645389</v>
+        <v>7.6870737075805664</v>
       </c>
       <c r="D223">
         <v>1</v>
@@ -3572,7 +3572,7 @@
         <v>1089</v>
       </c>
       <c r="C224">
-        <v>0.46981525421142578</v>
+        <v>0.29524350166320801</v>
       </c>
       <c r="D224">
         <v>1</v>
@@ -3586,7 +3586,7 @@
         <v>9478</v>
       </c>
       <c r="C225">
-        <v>13.81523728370667</v>
+        <v>9.7746143341064453</v>
       </c>
       <c r="D225">
         <v>1</v>
@@ -3600,7 +3600,7 @@
         <v>3351</v>
       </c>
       <c r="C226">
-        <v>2.8682293891906738</v>
+        <v>2.0108926296234131</v>
       </c>
       <c r="D226">
         <v>1</v>
@@ -3614,7 +3614,7 @@
         <v>9283</v>
       </c>
       <c r="C227">
-        <v>13.86517381668091</v>
+        <v>9.7152695655822754</v>
       </c>
       <c r="D227">
         <v>1</v>
@@ -3625,13 +3625,13 @@
         <v>226</v>
       </c>
       <c r="B228">
-        <v>21421</v>
+        <v>23555</v>
       </c>
       <c r="C228">
-        <v>60.003118515014648</v>
+        <v>50.184215784072883</v>
       </c>
       <c r="D228">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.35">
@@ -3642,7 +3642,7 @@
         <v>4098</v>
       </c>
       <c r="C229">
-        <v>3.7099752426147461</v>
+        <v>2.3618195056915279</v>
       </c>
       <c r="D229">
         <v>1</v>
@@ -3656,7 +3656,7 @@
         <v>6334</v>
       </c>
       <c r="C230">
-        <v>6.4122011661529541</v>
+        <v>4.5155489444732666</v>
       </c>
       <c r="D230">
         <v>1</v>
@@ -3670,7 +3670,7 @@
         <v>4002</v>
       </c>
       <c r="C231">
-        <v>3.674492359161377</v>
+        <v>2.4531013965606689</v>
       </c>
       <c r="D231">
         <v>1</v>
@@ -3684,7 +3684,7 @@
         <v>8028</v>
       </c>
       <c r="C232">
-        <v>11.20481848716736</v>
+        <v>7.0340001583099374</v>
       </c>
       <c r="D232">
         <v>1</v>
@@ -3698,7 +3698,7 @@
         <v>511</v>
       </c>
       <c r="C233">
-        <v>0.22892045974731451</v>
+        <v>0.1745448112487793</v>
       </c>
       <c r="D233">
         <v>1</v>
@@ -3712,7 +3712,7 @@
         <v>4305</v>
       </c>
       <c r="C234">
-        <v>4.348257303237915</v>
+        <v>2.6897456645965581</v>
       </c>
       <c r="D234">
         <v>1</v>
@@ -3726,7 +3726,7 @@
         <v>4993</v>
       </c>
       <c r="C235">
-        <v>5.095055103302002</v>
+        <v>3.4316642284393311</v>
       </c>
       <c r="D235">
         <v>1</v>
@@ -3740,7 +3740,7 @@
         <v>706</v>
       </c>
       <c r="C236">
-        <v>0.36130309104919428</v>
+        <v>0.27280950546264648</v>
       </c>
       <c r="D236">
         <v>1</v>
@@ -3754,7 +3754,7 @@
         <v>8314</v>
       </c>
       <c r="C237">
-        <v>11.211873054504389</v>
+        <v>7.6036982536315918</v>
       </c>
       <c r="D237">
         <v>1</v>
@@ -3768,7 +3768,7 @@
         <v>4122</v>
       </c>
       <c r="C238">
-        <v>3.2312774658203121</v>
+        <v>2.2644145488739009</v>
       </c>
       <c r="D238">
         <v>1</v>
@@ -3782,7 +3782,7 @@
         <v>20437</v>
       </c>
       <c r="C239">
-        <v>53.151732444763176</v>
+        <v>38.571435213088989</v>
       </c>
       <c r="D239">
         <v>1</v>
@@ -3796,7 +3796,7 @@
         <v>8045</v>
       </c>
       <c r="C240">
-        <v>9.9435756206512451</v>
+        <v>6.8674349784851074</v>
       </c>
       <c r="D240">
         <v>1</v>
@@ -3810,7 +3810,7 @@
         <v>747</v>
       </c>
       <c r="C241">
-        <v>0.48629546165466309</v>
+        <v>0.34301161766052252</v>
       </c>
       <c r="D241">
         <v>1</v>
@@ -3824,7 +3824,7 @@
         <v>1157</v>
       </c>
       <c r="C242">
-        <v>0.53328180313110352</v>
+        <v>0.37163567543029791</v>
       </c>
       <c r="D242">
         <v>1</v>
@@ -3838,7 +3838,7 @@
         <v>6478</v>
       </c>
       <c r="C243">
-        <v>6.9097769260406494</v>
+        <v>4.7228169441223136</v>
       </c>
       <c r="D243">
         <v>1</v>
@@ -3852,7 +3852,7 @@
         <v>6809</v>
       </c>
       <c r="C244">
-        <v>6.5130898952484131</v>
+        <v>4.339688777923584</v>
       </c>
       <c r="D244">
         <v>1</v>
@@ -3866,7 +3866,7 @@
         <v>12019</v>
       </c>
       <c r="C245">
-        <v>20.149695158004761</v>
+        <v>13.745670318603519</v>
       </c>
       <c r="D245">
         <v>1</v>
@@ -3880,7 +3880,7 @@
         <v>1771</v>
       </c>
       <c r="C246">
-        <v>1.196499109268188</v>
+        <v>0.94044089317321777</v>
       </c>
       <c r="D246">
         <v>1</v>
@@ -3894,7 +3894,7 @@
         <v>7726</v>
       </c>
       <c r="C247">
-        <v>9.9946048259735107</v>
+        <v>7.3263652324676514</v>
       </c>
       <c r="D247">
         <v>1</v>
@@ -3908,7 +3908,7 @@
         <v>3887</v>
       </c>
       <c r="C248">
-        <v>3.5114319324493408</v>
+        <v>2.7032196521759029</v>
       </c>
       <c r="D248">
         <v>1</v>
@@ -3922,7 +3922,7 @@
         <v>11623</v>
       </c>
       <c r="C249">
-        <v>19.47033262252808</v>
+        <v>13.80415940284729</v>
       </c>
       <c r="D249">
         <v>1</v>
@@ -3936,7 +3936,7 @@
         <v>9558</v>
       </c>
       <c r="C250">
-        <v>12.757875919342039</v>
+        <v>8.711540699005127</v>
       </c>
       <c r="D250">
         <v>1</v>
@@ -3950,7 +3950,7 @@
         <v>1406</v>
       </c>
       <c r="C251">
-        <v>0.66813015937805176</v>
+        <v>0.49716281890869141</v>
       </c>
       <c r="D251">
         <v>1</v>
@@ -3964,7 +3964,7 @@
         <v>5346</v>
       </c>
       <c r="C252">
-        <v>4.4541077613830566</v>
+        <v>3.22569727897644</v>
       </c>
       <c r="D252">
         <v>1</v>
@@ -3978,7 +3978,7 @@
         <v>7336</v>
       </c>
       <c r="C253">
-        <v>8.5755956172943115</v>
+        <v>8.0719499588012695</v>
       </c>
       <c r="D253">
         <v>1</v>
@@ -3992,7 +3992,7 @@
         <v>929</v>
       </c>
       <c r="C254">
-        <v>0.60872149467468262</v>
+        <v>0.40086221694946289</v>
       </c>
       <c r="D254">
         <v>1</v>
@@ -4006,7 +4006,7 @@
         <v>3108</v>
       </c>
       <c r="C255">
-        <v>2.4365770816802979</v>
+        <v>1.6690464019775391</v>
       </c>
       <c r="D255">
         <v>1</v>
@@ -4020,7 +4020,7 @@
         <v>987</v>
       </c>
       <c r="C256">
-        <v>0.36103129386901861</v>
+        <v>0.30356550216674799</v>
       </c>
       <c r="D256">
         <v>1</v>
@@ -4034,7 +4034,7 @@
         <v>4472</v>
       </c>
       <c r="C257">
-        <v>4.1925113201141357</v>
+        <v>3.398208856582642</v>
       </c>
       <c r="D257">
         <v>1</v>
@@ -4048,7 +4048,7 @@
         <v>5488</v>
       </c>
       <c r="C258">
-        <v>5.8620970249176034</v>
+        <v>4.8560030460357666</v>
       </c>
       <c r="D258">
         <v>1</v>
@@ -4062,7 +4062,7 @@
         <v>1030</v>
       </c>
       <c r="C259">
-        <v>0.58461689949035645</v>
+        <v>0.45674777030944819</v>
       </c>
       <c r="D259">
         <v>1</v>
@@ -4076,7 +4076,7 @@
         <v>4794</v>
       </c>
       <c r="C260">
-        <v>3.2608919143676758</v>
+        <v>2.370518684387207</v>
       </c>
       <c r="D260">
         <v>1</v>
@@ -4090,7 +4090,7 @@
         <v>1360</v>
       </c>
       <c r="C261">
-        <v>0.76169109344482422</v>
+        <v>0.52228760719299316</v>
       </c>
       <c r="D261">
         <v>1</v>
@@ -4104,7 +4104,7 @@
         <v>10676</v>
       </c>
       <c r="C262">
-        <v>14.96937417984009</v>
+        <v>11.586599349975589</v>
       </c>
       <c r="D262">
         <v>1</v>
@@ -4118,7 +4118,7 @@
         <v>5666</v>
       </c>
       <c r="C263">
-        <v>5.7532501220703116</v>
+        <v>4.7412009239196777</v>
       </c>
       <c r="D263">
         <v>1</v>
@@ -4132,7 +4132,7 @@
         <v>9316</v>
       </c>
       <c r="C264">
-        <v>14.26038527488708</v>
+        <v>10.936226367950439</v>
       </c>
       <c r="D264">
         <v>1</v>
@@ -4146,7 +4146,7 @@
         <v>5789</v>
       </c>
       <c r="C265">
-        <v>5.7080812454223633</v>
+        <v>4.4678540229797363</v>
       </c>
       <c r="D265">
         <v>1</v>
@@ -4157,10 +4157,10 @@
         <v>264</v>
       </c>
       <c r="B266">
-        <v>22052</v>
+        <v>25053</v>
       </c>
       <c r="C266">
-        <v>60.001443386077881</v>
+        <v>60.003024101257317</v>
       </c>
       <c r="D266">
         <v>0</v>
@@ -4174,7 +4174,7 @@
         <v>7993</v>
       </c>
       <c r="C267">
-        <v>9.304133415222168</v>
+        <v>7.0925354957580566</v>
       </c>
       <c r="D267">
         <v>1</v>
@@ -4188,7 +4188,7 @@
         <v>4653</v>
       </c>
       <c r="C268">
-        <v>3.906724214553833</v>
+        <v>3.052749872207642</v>
       </c>
       <c r="D268">
         <v>1</v>
@@ -4202,7 +4202,7 @@
         <v>2765</v>
       </c>
       <c r="C269">
-        <v>1.9213826656341551</v>
+        <v>1.416789293289185</v>
       </c>
       <c r="D269">
         <v>1</v>
@@ -4216,7 +4216,7 @@
         <v>2235</v>
       </c>
       <c r="C270">
-        <v>1.155729293823242</v>
+        <v>0.89969396591186523</v>
       </c>
       <c r="D270">
         <v>1</v>
@@ -4230,7 +4230,7 @@
         <v>14262</v>
       </c>
       <c r="C271">
-        <v>25.69376015663147</v>
+        <v>21.427693843841549</v>
       </c>
       <c r="D271">
         <v>1</v>
@@ -4244,7 +4244,7 @@
         <v>1339</v>
       </c>
       <c r="C272">
-        <v>0.54554510116577148</v>
+        <v>0.49663448333740229</v>
       </c>
       <c r="D272">
         <v>1</v>
@@ -4258,7 +4258,7 @@
         <v>15188</v>
       </c>
       <c r="C273">
-        <v>27.817575454711911</v>
+        <v>23.69496846199036</v>
       </c>
       <c r="D273">
         <v>1</v>
@@ -4272,7 +4272,7 @@
         <v>9504</v>
       </c>
       <c r="C274">
-        <v>12.761175870895389</v>
+        <v>10.50045824050903</v>
       </c>
       <c r="D274">
         <v>1</v>
@@ -4286,7 +4286,7 @@
         <v>3972</v>
       </c>
       <c r="C275">
-        <v>3.064801931381226</v>
+        <v>2.626878976821899</v>
       </c>
       <c r="D275">
         <v>1</v>
@@ -4300,7 +4300,7 @@
         <v>9588</v>
       </c>
       <c r="C276">
-        <v>11.589097261428829</v>
+        <v>9.2376136779785156</v>
       </c>
       <c r="D276">
         <v>1</v>
@@ -4314,7 +4314,7 @@
         <v>6689</v>
       </c>
       <c r="C277">
-        <v>7.0160295963287354</v>
+        <v>6.7713477611541748</v>
       </c>
       <c r="D277">
         <v>1</v>
@@ -4328,7 +4328,7 @@
         <v>4112</v>
       </c>
       <c r="C278">
-        <v>3.23063063621521</v>
+        <v>2.8301916122436519</v>
       </c>
       <c r="D278">
         <v>1</v>
@@ -4342,7 +4342,7 @@
         <v>3248</v>
       </c>
       <c r="C279">
-        <v>2.091094017028809</v>
+        <v>1.8550693988800051</v>
       </c>
       <c r="D279">
         <v>1</v>
@@ -4356,7 +4356,7 @@
         <v>3816</v>
       </c>
       <c r="C280">
-        <v>2.8769264221191411</v>
+        <v>2.355343341827393</v>
       </c>
       <c r="D280">
         <v>1</v>
@@ -4370,7 +4370,7 @@
         <v>4850</v>
       </c>
       <c r="C281">
-        <v>4.024465799331665</v>
+        <v>3.203450202941895</v>
       </c>
       <c r="D281">
         <v>1</v>
@@ -4384,7 +4384,7 @@
         <v>2659</v>
       </c>
       <c r="C282">
-        <v>1.451950788497925</v>
+        <v>1.279846668243408</v>
       </c>
       <c r="D282">
         <v>1</v>
@@ -4395,13 +4395,13 @@
         <v>281</v>
       </c>
       <c r="B283">
-        <v>23680</v>
+        <v>24527</v>
       </c>
       <c r="C283">
-        <v>60.003885269165039</v>
+        <v>55.609020709991462</v>
       </c>
       <c r="D283">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.35">
@@ -4412,7 +4412,7 @@
         <v>4768</v>
       </c>
       <c r="C284">
-        <v>3.557847261428833</v>
+        <v>3.208128690719604</v>
       </c>
       <c r="D284">
         <v>1</v>
@@ -4426,7 +4426,7 @@
         <v>20440</v>
       </c>
       <c r="C285">
-        <v>44.865357637405403</v>
+        <v>38.825459480285637</v>
       </c>
       <c r="D285">
         <v>1</v>
@@ -4440,7 +4440,7 @@
         <v>8797</v>
       </c>
       <c r="C286">
-        <v>9.4742698669433594</v>
+        <v>8.2772603034973145</v>
       </c>
       <c r="D286">
         <v>1</v>
@@ -4454,7 +4454,7 @@
         <v>2003</v>
       </c>
       <c r="C287">
-        <v>1.031277656555176</v>
+        <v>0.88346600532531738</v>
       </c>
       <c r="D287">
         <v>1</v>
@@ -4468,7 +4468,7 @@
         <v>8417</v>
       </c>
       <c r="C288">
-        <v>9.8845510482788086</v>
+        <v>7.8137948513031006</v>
       </c>
       <c r="D288">
         <v>1</v>
@@ -4482,7 +4482,7 @@
         <v>2907</v>
       </c>
       <c r="C289">
-        <v>1.4794836044311519</v>
+        <v>1.306690454483032</v>
       </c>
       <c r="D289">
         <v>1</v>
@@ -4493,10 +4493,10 @@
         <v>288</v>
       </c>
       <c r="B290">
-        <v>26314</v>
+        <v>26792</v>
       </c>
       <c r="C290">
-        <v>60.005749940872192</v>
+        <v>60.004565477371223</v>
       </c>
       <c r="D290">
         <v>0</v>
@@ -4510,7 +4510,7 @@
         <v>7825</v>
       </c>
       <c r="C291">
-        <v>6.2233469486236572</v>
+        <v>6.0642998218536377</v>
       </c>
       <c r="D291">
         <v>1</v>
@@ -4524,7 +4524,7 @@
         <v>2062</v>
       </c>
       <c r="C292">
-        <v>0.79807353019714355</v>
+        <v>0.75666046142578125</v>
       </c>
       <c r="D292">
         <v>1</v>
@@ -4538,7 +4538,7 @@
         <v>1062</v>
       </c>
       <c r="C293">
-        <v>0.39395380020141602</v>
+        <v>0.38488316535949713</v>
       </c>
       <c r="D293">
         <v>1</v>
@@ -4552,7 +4552,7 @@
         <v>3184</v>
       </c>
       <c r="C294">
-        <v>1.22325587272644</v>
+        <v>1.201053380966187</v>
       </c>
       <c r="D294">
         <v>1</v>
@@ -4566,7 +4566,7 @@
         <v>2417</v>
       </c>
       <c r="C295">
-        <v>0.9542689323425293</v>
+        <v>0.87607765197753906</v>
       </c>
       <c r="D295">
         <v>1</v>
@@ -4580,7 +4580,7 @@
         <v>6241</v>
       </c>
       <c r="C296">
-        <v>3.9626984596252441</v>
+        <v>3.969612598419189</v>
       </c>
       <c r="D296">
         <v>1</v>
@@ -4594,7 +4594,7 @@
         <v>4784</v>
       </c>
       <c r="C297">
-        <v>2.7608845233917241</v>
+        <v>2.7086431980133061</v>
       </c>
       <c r="D297">
         <v>1</v>
@@ -4608,7 +4608,7 @@
         <v>1820</v>
       </c>
       <c r="C298">
-        <v>0.70655655860900879</v>
+        <v>0.69681787490844727</v>
       </c>
       <c r="D298">
         <v>1</v>
@@ -4622,7 +4622,7 @@
         <v>2265</v>
       </c>
       <c r="C299">
-        <v>0.91398215293884277</v>
+        <v>0.89609098434448242</v>
       </c>
       <c r="D299">
         <v>1</v>
@@ -4636,7 +4636,7 @@
         <v>3153</v>
       </c>
       <c r="C300">
-        <v>1.341678380966187</v>
+        <v>1.2962827682495119</v>
       </c>
       <c r="D300">
         <v>1</v>
@@ -4650,7 +4650,7 @@
         <v>1529</v>
       </c>
       <c r="C301">
-        <v>0.57245492935180664</v>
+        <v>0.56072592735290527</v>
       </c>
       <c r="D301">
         <v>1</v>
@@ -4664,7 +4664,7 @@
         <v>7875</v>
       </c>
       <c r="C302">
-        <v>9.2165358066558838</v>
+        <v>7.9141747951507568</v>
       </c>
       <c r="D302">
         <v>1</v>
@@ -4678,7 +4678,7 @@
         <v>1992</v>
       </c>
       <c r="C303">
-        <v>1.520934104919434</v>
+        <v>1.1775074005126951</v>
       </c>
       <c r="D303">
         <v>1</v>
@@ -4692,7 +4692,7 @@
         <v>2325</v>
       </c>
       <c r="C304">
-        <v>1.514836311340332</v>
+        <v>1.2526941299438481</v>
       </c>
       <c r="D304">
         <v>1</v>
@@ -4706,7 +4706,7 @@
         <v>1545</v>
       </c>
       <c r="C305">
-        <v>0.73075962066650391</v>
+        <v>0.65624308586120605</v>
       </c>
       <c r="D305">
         <v>1</v>
@@ -4720,7 +4720,7 @@
         <v>6373</v>
       </c>
       <c r="C306">
-        <v>8.059009313583374</v>
+        <v>6.5421888828277588</v>
       </c>
       <c r="D306">
         <v>1</v>
@@ -4734,7 +4734,7 @@
         <v>1395</v>
       </c>
       <c r="C307">
-        <v>0.589385986328125</v>
+        <v>0.53186941146850586</v>
       </c>
       <c r="D307">
         <v>1</v>
@@ -4748,7 +4748,7 @@
         <v>2483</v>
       </c>
       <c r="C308">
-        <v>1.8335120677948</v>
+        <v>1.53418493270874</v>
       </c>
       <c r="D308">
         <v>1</v>
@@ -4762,7 +4762,7 @@
         <v>8012</v>
       </c>
       <c r="C309">
-        <v>8.6824758052825928</v>
+        <v>7.2178404331207284</v>
       </c>
       <c r="D309">
         <v>1</v>
@@ -4776,7 +4776,7 @@
         <v>991</v>
       </c>
       <c r="C310">
-        <v>0.42144179344177252</v>
+        <v>0.3791201114654541</v>
       </c>
       <c r="D310">
         <v>1</v>
@@ -4790,7 +4790,7 @@
         <v>3278</v>
       </c>
       <c r="C311">
-        <v>2.6636018753051758</v>
+        <v>2.2095978260040279</v>
       </c>
       <c r="D311">
         <v>1</v>
@@ -4804,7 +4804,7 @@
         <v>5043</v>
       </c>
       <c r="C312">
-        <v>4.6377005577087402</v>
+        <v>3.8901090621948242</v>
       </c>
       <c r="D312">
         <v>1</v>
@@ -4818,7 +4818,7 @@
         <v>15349</v>
       </c>
       <c r="C313">
-        <v>25.976904392242432</v>
+        <v>21.41181588172913</v>
       </c>
       <c r="D313">
         <v>1</v>
@@ -4832,7 +4832,7 @@
         <v>4893</v>
       </c>
       <c r="C314">
-        <v>4.8957381248474121</v>
+        <v>3.9871141910552979</v>
       </c>
       <c r="D314">
         <v>1</v>
@@ -4846,7 +4846,7 @@
         <v>10091</v>
       </c>
       <c r="C315">
-        <v>12.71672344207764</v>
+        <v>10.009110927581791</v>
       </c>
       <c r="D315">
         <v>1</v>
@@ -4860,7 +4860,7 @@
         <v>11580</v>
       </c>
       <c r="C316">
-        <v>18.29907584190369</v>
+        <v>13.57191133499146</v>
       </c>
       <c r="D316">
         <v>1</v>
@@ -4874,7 +4874,7 @@
         <v>8226</v>
       </c>
       <c r="C317">
-        <v>10.950275182724001</v>
+        <v>8.0613939762115479</v>
       </c>
       <c r="D317">
         <v>1</v>
@@ -4888,7 +4888,7 @@
         <v>13535</v>
       </c>
       <c r="C318">
-        <v>25.592559814453121</v>
+        <v>20.2875030040741</v>
       </c>
       <c r="D318">
         <v>1</v>
@@ -4902,7 +4902,7 @@
         <v>7497</v>
       </c>
       <c r="C319">
-        <v>9.3522412776947021</v>
+        <v>6.6248657703399658</v>
       </c>
       <c r="D319">
         <v>1</v>
@@ -4916,7 +4916,7 @@
         <v>8761</v>
       </c>
       <c r="C320">
-        <v>11.98254489898682</v>
+        <v>8.5370948314666748</v>
       </c>
       <c r="D320">
         <v>1</v>
@@ -4930,7 +4930,7 @@
         <v>14242</v>
       </c>
       <c r="C321">
-        <v>30.486166000366211</v>
+        <v>21.559669256210331</v>
       </c>
       <c r="D321">
         <v>1</v>
@@ -4944,7 +4944,7 @@
         <v>2234</v>
       </c>
       <c r="C322">
-        <v>1.546484231948853</v>
+        <v>1.1469676494598391</v>
       </c>
       <c r="D322">
         <v>1</v>
@@ -4958,7 +4958,7 @@
         <v>5640</v>
       </c>
       <c r="C323">
-        <v>5.5506227016448966</v>
+        <v>3.9640531539916992</v>
       </c>
       <c r="D323">
         <v>1</v>
@@ -4972,7 +4972,7 @@
         <v>2687</v>
       </c>
       <c r="C324">
-        <v>2.1382396221160889</v>
+        <v>1.4823422431945801</v>
       </c>
       <c r="D324">
         <v>1</v>
@@ -4986,7 +4986,7 @@
         <v>8255</v>
       </c>
       <c r="C325">
-        <v>11.22588801383972</v>
+        <v>7.7926578521728516</v>
       </c>
       <c r="D325">
         <v>1</v>
@@ -5000,7 +5000,7 @@
         <v>7685</v>
       </c>
       <c r="C326">
-        <v>9.9849278926849365</v>
+        <v>7.2907557487487793</v>
       </c>
       <c r="D326">
         <v>1</v>
@@ -5014,7 +5014,7 @@
         <v>2654</v>
       </c>
       <c r="C327">
-        <v>2.0033154487609859</v>
+        <v>1.4930529594421389</v>
       </c>
       <c r="D327">
         <v>1</v>
@@ -5028,7 +5028,7 @@
         <v>1177</v>
       </c>
       <c r="C328">
-        <v>0.67146635055541992</v>
+        <v>0.55144858360290527</v>
       </c>
       <c r="D328">
         <v>1</v>
@@ -5042,7 +5042,7 @@
         <v>10092</v>
       </c>
       <c r="C329">
-        <v>14.436088085174561</v>
+        <v>10.46492910385132</v>
       </c>
       <c r="D329">
         <v>1</v>
@@ -5056,7 +5056,7 @@
         <v>109</v>
       </c>
       <c r="C330">
-        <v>5.7879447937011719E-2</v>
+        <v>4.4213533401489258E-2</v>
       </c>
       <c r="D330">
         <v>1</v>
@@ -5070,7 +5070,7 @@
         <v>3363</v>
       </c>
       <c r="C331">
-        <v>2.5689849853515621</v>
+        <v>1.750082731246948</v>
       </c>
       <c r="D331">
         <v>1</v>
@@ -5081,10 +5081,10 @@
         <v>330</v>
       </c>
       <c r="B332">
-        <v>21823</v>
+        <v>26608</v>
       </c>
       <c r="C332">
-        <v>60.000155925750732</v>
+        <v>60.001578807830811</v>
       </c>
       <c r="D332">
         <v>0</v>
@@ -5098,7 +5098,7 @@
         <v>4802</v>
       </c>
       <c r="C333">
-        <v>4.7138960361480713</v>
+        <v>3.1124751567840581</v>
       </c>
       <c r="D333">
         <v>1</v>
@@ -5112,7 +5112,7 @@
         <v>3908</v>
       </c>
       <c r="C334">
-        <v>3.6357016563415532</v>
+        <v>2.4932057857513432</v>
       </c>
       <c r="D334">
         <v>1</v>
@@ -5126,7 +5126,7 @@
         <v>3327</v>
       </c>
       <c r="C335">
-        <v>2.6539313793182369</v>
+        <v>1.775290966033936</v>
       </c>
       <c r="D335">
         <v>1</v>
@@ -5140,7 +5140,7 @@
         <v>1411</v>
       </c>
       <c r="C336">
-        <v>0.97425675392150879</v>
+        <v>0.58553838729858398</v>
       </c>
       <c r="D336">
         <v>1</v>
@@ -5154,7 +5154,7 @@
         <v>767</v>
       </c>
       <c r="C337">
-        <v>0.34805774688720698</v>
+        <v>0.25136828422546392</v>
       </c>
       <c r="D337">
         <v>1</v>
@@ -5168,7 +5168,7 @@
         <v>7409</v>
       </c>
       <c r="C338">
-        <v>7.4461147785186768</v>
+        <v>5.2965848445892334</v>
       </c>
       <c r="D338">
         <v>1</v>
@@ -5182,7 +5182,7 @@
         <v>3525</v>
       </c>
       <c r="C339">
-        <v>1.1266715526580811</v>
+        <v>0.83959317207336426</v>
       </c>
       <c r="D339">
         <v>1</v>
@@ -5196,7 +5196,7 @@
         <v>5568</v>
       </c>
       <c r="C340">
-        <v>5.5830631256103516</v>
+        <v>3.8294463157653809</v>
       </c>
       <c r="D340">
         <v>1</v>
@@ -5210,7 +5210,7 @@
         <v>5988</v>
       </c>
       <c r="C341">
-        <v>6.3184568881988534</v>
+        <v>4.176910400390625</v>
       </c>
       <c r="D341">
         <v>1</v>
@@ -5224,7 +5224,7 @@
         <v>19066</v>
       </c>
       <c r="C342">
-        <v>48.925544500350952</v>
+        <v>35.938483953475952</v>
       </c>
       <c r="D342">
         <v>1</v>
@@ -5238,7 +5238,7 @@
         <v>4771</v>
       </c>
       <c r="C343">
-        <v>4.803424596786499</v>
+        <v>3.1229796409606929</v>
       </c>
       <c r="D343">
         <v>1</v>
@@ -5252,7 +5252,7 @@
         <v>10717</v>
       </c>
       <c r="C344">
-        <v>15.96044969558716</v>
+        <v>12.06258964538574</v>
       </c>
       <c r="D344">
         <v>1</v>
@@ -5266,7 +5266,7 @@
         <v>1912</v>
       </c>
       <c r="C345">
-        <v>1.4492330551147461</v>
+        <v>0.88266801834106445</v>
       </c>
       <c r="D345">
         <v>1</v>
@@ -5280,7 +5280,7 @@
         <v>8821</v>
       </c>
       <c r="C346">
-        <v>12.337765693664551</v>
+        <v>8.9626784324645996</v>
       </c>
       <c r="D346">
         <v>1</v>
@@ -5294,7 +5294,7 @@
         <v>8140</v>
       </c>
       <c r="C347">
-        <v>8.1145217418670654</v>
+        <v>5.8027138710021973</v>
       </c>
       <c r="D347">
         <v>1</v>
@@ -5308,7 +5308,7 @@
         <v>8334</v>
       </c>
       <c r="C348">
-        <v>9.8834939002990723</v>
+        <v>7.1828036308288574</v>
       </c>
       <c r="D348">
         <v>1</v>
@@ -5322,7 +5322,7 @@
         <v>5072</v>
       </c>
       <c r="C349">
-        <v>4.3887534141540527</v>
+        <v>2.6738109588623051</v>
       </c>
       <c r="D349">
         <v>1</v>
@@ -5336,7 +5336,7 @@
         <v>1622</v>
       </c>
       <c r="C350">
-        <v>0.92786931991577148</v>
+        <v>0.79530501365661621</v>
       </c>
       <c r="D350">
         <v>1</v>
@@ -5350,7 +5350,7 @@
         <v>3809</v>
       </c>
       <c r="C351">
-        <v>2.1676335334777832</v>
+        <v>1.570146799087524</v>
       </c>
       <c r="D351">
         <v>1</v>
@@ -5364,7 +5364,7 @@
         <v>2818</v>
       </c>
       <c r="C352">
-        <v>2.0005125999450679</v>
+        <v>1.459342956542969</v>
       </c>
       <c r="D352">
         <v>1</v>
@@ -5378,7 +5378,7 @@
         <v>3726</v>
       </c>
       <c r="C353">
-        <v>2.934284925460815</v>
+        <v>2.0808005332946782</v>
       </c>
       <c r="D353">
         <v>1</v>
@@ -5392,7 +5392,7 @@
         <v>11179</v>
       </c>
       <c r="C354">
-        <v>16.667028188705441</v>
+        <v>14.169003486633301</v>
       </c>
       <c r="D354">
         <v>1</v>
@@ -5406,7 +5406,7 @@
         <v>2381</v>
       </c>
       <c r="C355">
-        <v>1.212937116622925</v>
+        <v>0.95129108428955078</v>
       </c>
       <c r="D355">
         <v>1</v>
@@ -5420,7 +5420,7 @@
         <v>9612</v>
       </c>
       <c r="C356">
-        <v>14.03315758705139</v>
+        <v>10.429489612579349</v>
       </c>
       <c r="D356">
         <v>1</v>
@@ -5434,7 +5434,7 @@
         <v>534</v>
       </c>
       <c r="C357">
-        <v>0.29367637634277338</v>
+        <v>0.18202924728393549</v>
       </c>
       <c r="D357">
         <v>1</v>
@@ -5448,7 +5448,7 @@
         <v>11967</v>
       </c>
       <c r="C358">
-        <v>20.344071388244629</v>
+        <v>15.676165342330931</v>
       </c>
       <c r="D358">
         <v>1</v>
@@ -5459,10 +5459,10 @@
         <v>357</v>
       </c>
       <c r="B359">
-        <v>21676</v>
+        <v>24782</v>
       </c>
       <c r="C359">
-        <v>60.005682945251458</v>
+        <v>60.002544641494751</v>
       </c>
       <c r="D359">
         <v>0</v>
@@ -5476,7 +5476,7 @@
         <v>3062</v>
       </c>
       <c r="C360">
-        <v>2.2924025058746338</v>
+        <v>1.770901203155518</v>
       </c>
       <c r="D360">
         <v>1</v>
@@ -5490,7 +5490,7 @@
         <v>695</v>
       </c>
       <c r="C361">
-        <v>0.34047436714172358</v>
+        <v>0.27638840675353998</v>
       </c>
       <c r="D361">
         <v>1</v>
@@ -5504,7 +5504,7 @@
         <v>6960</v>
       </c>
       <c r="C362">
-        <v>8.00534987449646</v>
+        <v>6.2512667179107666</v>
       </c>
       <c r="D362">
         <v>1</v>
@@ -5518,7 +5518,7 @@
         <v>585</v>
       </c>
       <c r="C363">
-        <v>0.29179286956787109</v>
+        <v>0.19952511787414551</v>
       </c>
       <c r="D363">
         <v>1</v>
@@ -5532,7 +5532,7 @@
         <v>10370</v>
       </c>
       <c r="C364">
-        <v>16.228446245193481</v>
+        <v>11.73479962348938</v>
       </c>
       <c r="D364">
         <v>1</v>
@@ -5546,7 +5546,7 @@
         <v>2220</v>
       </c>
       <c r="C365">
-        <v>1.45068883895874</v>
+        <v>1.128860235214233</v>
       </c>
       <c r="D365">
         <v>1</v>
@@ -5560,7 +5560,7 @@
         <v>623</v>
       </c>
       <c r="C366">
-        <v>0.32811808586120611</v>
+        <v>0.23300790786743161</v>
       </c>
       <c r="D366">
         <v>1</v>
@@ -5574,7 +5574,7 @@
         <v>1098</v>
       </c>
       <c r="C367">
-        <v>0.64034843444824219</v>
+        <v>0.46468186378478998</v>
       </c>
       <c r="D367">
         <v>1</v>
@@ -5588,7 +5588,7 @@
         <v>794</v>
       </c>
       <c r="C368">
-        <v>0.39588689804077148</v>
+        <v>0.28825807571411127</v>
       </c>
       <c r="D368">
         <v>1</v>
@@ -5602,7 +5602,7 @@
         <v>4404</v>
       </c>
       <c r="C369">
-        <v>4.0067882537841797</v>
+        <v>2.9683747291564941</v>
       </c>
       <c r="D369">
         <v>1</v>
@@ -5616,7 +5616,7 @@
         <v>1041</v>
       </c>
       <c r="C370">
-        <v>0.53970575332641602</v>
+        <v>0.43696308135986328</v>
       </c>
       <c r="D370">
         <v>1</v>
@@ -5630,7 +5630,7 @@
         <v>796</v>
       </c>
       <c r="C371">
-        <v>0.3364417552947998</v>
+        <v>0.31552624702453608</v>
       </c>
       <c r="D371">
         <v>1</v>
@@ -5644,7 +5644,7 @@
         <v>15674</v>
       </c>
       <c r="C372">
-        <v>29.150876045227051</v>
+        <v>23.11936092376709</v>
       </c>
       <c r="D372">
         <v>1</v>
@@ -5658,7 +5658,7 @@
         <v>3125</v>
       </c>
       <c r="C373">
-        <v>2.0815572738647461</v>
+        <v>1.5901451110839839</v>
       </c>
       <c r="D373">
         <v>1</v>
@@ -5672,7 +5672,7 @@
         <v>5201</v>
       </c>
       <c r="C374">
-        <v>4.6337025165557861</v>
+        <v>3.7441399097442631</v>
       </c>
       <c r="D374">
         <v>1</v>
@@ -5686,7 +5686,7 @@
         <v>14225</v>
       </c>
       <c r="C375">
-        <v>23.342267036437988</v>
+        <v>20.66100978851318</v>
       </c>
       <c r="D375">
         <v>1</v>
@@ -5700,7 +5700,7 @@
         <v>199</v>
       </c>
       <c r="C376">
-        <v>9.4042301177978516E-2</v>
+        <v>7.3812007904052734E-2</v>
       </c>
       <c r="D376">
         <v>1</v>
@@ -5714,7 +5714,7 @@
         <v>1514</v>
       </c>
       <c r="C377">
-        <v>0.88782596588134766</v>
+        <v>0.72510457038879395</v>
       </c>
       <c r="D377">
         <v>1</v>
@@ -5728,7 +5728,7 @@
         <v>14134</v>
       </c>
       <c r="C378">
-        <v>22.852586269378659</v>
+        <v>20.41955208778381</v>
       </c>
       <c r="D378">
         <v>1</v>
@@ -5742,7 +5742,7 @@
         <v>3161</v>
       </c>
       <c r="C379">
-        <v>2.1576094627380371</v>
+        <v>2.4004874229431148</v>
       </c>
       <c r="D379">
         <v>1</v>
@@ -5756,7 +5756,7 @@
         <v>8951</v>
       </c>
       <c r="C380">
-        <v>10.332931518554689</v>
+        <v>8.9948391914367676</v>
       </c>
       <c r="D380">
         <v>1</v>
@@ -5770,7 +5770,7 @@
         <v>5113</v>
       </c>
       <c r="C381">
-        <v>2.4876749515533452</v>
+        <v>2.0608599185943599</v>
       </c>
       <c r="D381">
         <v>1</v>
@@ -5784,7 +5784,7 @@
         <v>19374</v>
       </c>
       <c r="C382">
-        <v>38.496455669403083</v>
+        <v>33.595030546188347</v>
       </c>
       <c r="D382">
         <v>1</v>
@@ -5798,7 +5798,7 @@
         <v>20212</v>
       </c>
       <c r="C383">
-        <v>45.843476533889771</v>
+        <v>40.842596054077148</v>
       </c>
       <c r="D383">
         <v>1</v>
@@ -5812,7 +5812,7 @@
         <v>9252</v>
       </c>
       <c r="C384">
-        <v>10.30615901947021</v>
+        <v>8.9535946846008301</v>
       </c>
       <c r="D384">
         <v>1</v>
@@ -5826,7 +5826,7 @@
         <v>1906</v>
       </c>
       <c r="C385">
-        <v>0.9891362190246582</v>
+        <v>0.89001893997192383</v>
       </c>
       <c r="D385">
         <v>1</v>
@@ -5840,7 +5840,7 @@
         <v>4621</v>
       </c>
       <c r="C386">
-        <v>2.642607688903809</v>
+        <v>2.286929845809937</v>
       </c>
       <c r="D386">
         <v>1</v>
@@ -5854,7 +5854,7 @@
         <v>4470</v>
       </c>
       <c r="C387">
-        <v>3.49329686164856</v>
+        <v>2.687897682189941</v>
       </c>
       <c r="D387">
         <v>1</v>
@@ -5868,7 +5868,7 @@
         <v>9649</v>
       </c>
       <c r="C388">
-        <v>10.942130088806151</v>
+        <v>9.7632436752319336</v>
       </c>
       <c r="D388">
         <v>1</v>
@@ -5879,10 +5879,10 @@
         <v>387</v>
       </c>
       <c r="B389">
-        <v>24120</v>
+        <v>25387</v>
       </c>
       <c r="C389">
-        <v>60.000885486602783</v>
+        <v>60.000494480133057</v>
       </c>
       <c r="D389">
         <v>0</v>
@@ -5896,7 +5896,7 @@
         <v>12007</v>
       </c>
       <c r="C390">
-        <v>15.35252213478088</v>
+        <v>13.79620456695557</v>
       </c>
       <c r="D390">
         <v>1</v>
@@ -5910,7 +5910,7 @@
         <v>12388</v>
       </c>
       <c r="C391">
-        <v>16.13423919677734</v>
+        <v>13.899581432342529</v>
       </c>
       <c r="D391">
         <v>1</v>
@@ -5924,7 +5924,7 @@
         <v>8076</v>
       </c>
       <c r="C392">
-        <v>7.2270219326019287</v>
+        <v>6.2563779354095459</v>
       </c>
       <c r="D392">
         <v>1</v>
@@ -5938,7 +5938,7 @@
         <v>13788</v>
       </c>
       <c r="C393">
-        <v>16.514452219009399</v>
+        <v>15.16164970397949</v>
       </c>
       <c r="D393">
         <v>1</v>
@@ -5952,7 +5952,7 @@
         <v>3642</v>
       </c>
       <c r="C394">
-        <v>1.7023735046386721</v>
+        <v>1.6583588123321531</v>
       </c>
       <c r="D394">
         <v>1</v>
@@ -5966,7 +5966,7 @@
         <v>7256</v>
       </c>
       <c r="C395">
-        <v>5.0304157733917236</v>
+        <v>4.8503756523132324</v>
       </c>
       <c r="D395">
         <v>1</v>
@@ -5980,7 +5980,7 @@
         <v>682</v>
       </c>
       <c r="C396">
-        <v>0.20806789398193359</v>
+        <v>0.2005040645599365</v>
       </c>
       <c r="D396">
         <v>1</v>
@@ -5994,7 +5994,7 @@
         <v>6265</v>
       </c>
       <c r="C397">
-        <v>3.635694026947021</v>
+        <v>3.5363612174987789</v>
       </c>
       <c r="D397">
         <v>1</v>
@@ -6008,7 +6008,7 @@
         <v>3626</v>
       </c>
       <c r="C398">
-        <v>1.8754978179931641</v>
+        <v>1.8423559665679929</v>
       </c>
       <c r="D398">
         <v>1</v>
@@ -6022,7 +6022,7 @@
         <v>1688</v>
       </c>
       <c r="C399">
-        <v>0.63133978843688965</v>
+        <v>0.6145164966583252</v>
       </c>
       <c r="D399">
         <v>1</v>
@@ -6036,7 +6036,7 @@
         <v>2388</v>
       </c>
       <c r="C400">
-        <v>0.95793032646179199</v>
+        <v>0.91974377632141113</v>
       </c>
       <c r="D400">
         <v>1</v>
@@ -6050,7 +6050,7 @@
         <v>1836</v>
       </c>
       <c r="C401">
-        <v>0.58270120620727539</v>
+        <v>0.56229352951049805</v>
       </c>
       <c r="D401">
         <v>1</v>
@@ -6064,7 +6064,7 @@
         <v>14627</v>
       </c>
       <c r="C402">
-        <v>29.61960411071777</v>
+        <v>25.140612125396729</v>
       </c>
       <c r="D402">
         <v>1</v>
@@ -6078,7 +6078,7 @@
         <v>1233</v>
       </c>
       <c r="C403">
-        <v>0.75591850280761719</v>
+        <v>0.60891842842102051</v>
       </c>
       <c r="D403">
         <v>1</v>
@@ -6092,7 +6092,7 @@
         <v>1972</v>
       </c>
       <c r="C404">
-        <v>1.320070266723633</v>
+        <v>1.199352502822876</v>
       </c>
       <c r="D404">
         <v>1</v>
@@ -6106,7 +6106,7 @@
         <v>2804</v>
       </c>
       <c r="C405">
-        <v>1.833035469055176</v>
+        <v>1.3763449192047119</v>
       </c>
       <c r="D405">
         <v>1</v>
@@ -6120,7 +6120,7 @@
         <v>6613</v>
       </c>
       <c r="C406">
-        <v>7.8238668441772461</v>
+        <v>6.6877937316894531</v>
       </c>
       <c r="D406">
         <v>1</v>
@@ -6134,7 +6134,7 @@
         <v>6684</v>
       </c>
       <c r="C407">
-        <v>6.1763992309570313</v>
+        <v>4.6096427440643311</v>
       </c>
       <c r="D407">
         <v>1</v>
@@ -6148,7 +6148,7 @@
         <v>9944</v>
       </c>
       <c r="C408">
-        <v>12.85364747047424</v>
+        <v>11.157874345779421</v>
       </c>
       <c r="D408">
         <v>1</v>
@@ -6162,7 +6162,7 @@
         <v>4121</v>
       </c>
       <c r="C409">
-        <v>3.4597072601318359</v>
+        <v>3.0516452789306641</v>
       </c>
       <c r="D409">
         <v>1</v>
@@ -6173,10 +6173,10 @@
         <v>408</v>
       </c>
       <c r="B410">
-        <v>21914</v>
+        <v>24470</v>
       </c>
       <c r="C410">
-        <v>60.001121044158943</v>
+        <v>60.000593900680542</v>
       </c>
       <c r="D410">
         <v>0</v>
@@ -6190,7 +6190,7 @@
         <v>1057</v>
       </c>
       <c r="C411">
-        <v>0.66107559204101563</v>
+        <v>0.43899106979370123</v>
       </c>
       <c r="D411">
         <v>1</v>
@@ -6204,7 +6204,7 @@
         <v>4366</v>
       </c>
       <c r="C412">
-        <v>4.1404247283935547</v>
+        <v>2.8162870407104492</v>
       </c>
       <c r="D412">
         <v>1</v>
@@ -6218,7 +6218,7 @@
         <v>2701</v>
       </c>
       <c r="C413">
-        <v>1.8919496536254881</v>
+        <v>1.4179143905639651</v>
       </c>
       <c r="D413">
         <v>1</v>
@@ -6232,7 +6232,7 @@
         <v>11918</v>
       </c>
       <c r="C414">
-        <v>20.879692554473881</v>
+        <v>14.808429002761841</v>
       </c>
       <c r="D414">
         <v>1</v>
@@ -6246,7 +6246,7 @@
         <v>1961</v>
       </c>
       <c r="C415">
-        <v>1.5613865852355959</v>
+        <v>0.96471738815307617</v>
       </c>
       <c r="D415">
         <v>1</v>
@@ -6260,7 +6260,7 @@
         <v>5814</v>
       </c>
       <c r="C416">
-        <v>6.4521842002868652</v>
+        <v>4.5251433849334717</v>
       </c>
       <c r="D416">
         <v>1</v>
@@ -6274,7 +6274,7 @@
         <v>14488</v>
       </c>
       <c r="C417">
-        <v>27.827132701873779</v>
+        <v>20.710929393768311</v>
       </c>
       <c r="D417">
         <v>1</v>
@@ -6288,7 +6288,7 @@
         <v>2825</v>
       </c>
       <c r="C418">
-        <v>2.1283543109893799</v>
+        <v>1.45424485206604</v>
       </c>
       <c r="D418">
         <v>1</v>
@@ -6302,7 +6302,7 @@
         <v>3850</v>
       </c>
       <c r="C419">
-        <v>3.3656356334686279</v>
+        <v>2.2920644283294682</v>
       </c>
       <c r="D419">
         <v>1</v>
@@ -6316,7 +6316,7 @@
         <v>8822</v>
       </c>
       <c r="C420">
-        <v>11.92962384223938</v>
+        <v>8.3367419242858887</v>
       </c>
       <c r="D420">
         <v>1</v>
@@ -6330,7 +6330,7 @@
         <v>3526</v>
       </c>
       <c r="C421">
-        <v>2.8875606060028081</v>
+        <v>1.919137239456177</v>
       </c>
       <c r="D421">
         <v>1</v>
@@ -6344,7 +6344,7 @@
         <v>2662</v>
       </c>
       <c r="C422">
-        <v>1.9700801372528081</v>
+        <v>1.3370940685272219</v>
       </c>
       <c r="D422">
         <v>1</v>
@@ -6358,7 +6358,7 @@
         <v>3206</v>
       </c>
       <c r="C423">
-        <v>2.6831991672515869</v>
+        <v>1.678504467010498</v>
       </c>
       <c r="D423">
         <v>1</v>
@@ -6372,7 +6372,7 @@
         <v>5380</v>
       </c>
       <c r="C424">
-        <v>5.6866497993469238</v>
+        <v>3.7615752220153809</v>
       </c>
       <c r="D424">
         <v>1</v>
@@ -6386,7 +6386,7 @@
         <v>2518</v>
       </c>
       <c r="C425">
-        <v>1.7649950981140139</v>
+        <v>1.1976990699768071</v>
       </c>
       <c r="D425">
         <v>1</v>
@@ -6400,7 +6400,7 @@
         <v>3245</v>
       </c>
       <c r="C426">
-        <v>2.5236432552337651</v>
+        <v>1.5458447933197019</v>
       </c>
       <c r="D426">
         <v>1</v>
@@ -6414,7 +6414,7 @@
         <v>1802</v>
       </c>
       <c r="C427">
-        <v>0.90074467658996582</v>
+        <v>0.54465174674987793</v>
       </c>
       <c r="D427">
         <v>1</v>
@@ -6428,7 +6428,7 @@
         <v>7636</v>
       </c>
       <c r="C428">
-        <v>10.078855514526371</v>
+        <v>6.6098020076751709</v>
       </c>
       <c r="D428">
         <v>1</v>
@@ -6442,7 +6442,7 @@
         <v>7211</v>
       </c>
       <c r="C429">
-        <v>8.7013885974884033</v>
+        <v>5.916283130645752</v>
       </c>
       <c r="D429">
         <v>1</v>
@@ -6456,7 +6456,7 @@
         <v>1676</v>
       </c>
       <c r="C430">
-        <v>1.09430980682373</v>
+        <v>0.69094061851501465</v>
       </c>
       <c r="D430">
         <v>1</v>
@@ -6470,7 +6470,7 @@
         <v>6318</v>
       </c>
       <c r="C431">
-        <v>6.8134772777557373</v>
+        <v>4.7530815601348877</v>
       </c>
       <c r="D431">
         <v>1</v>
@@ -6484,7 +6484,7 @@
         <v>2829</v>
       </c>
       <c r="C432">
-        <v>1.521923303604126</v>
+        <v>1.048093795776367</v>
       </c>
       <c r="D432">
         <v>1</v>
@@ -6498,7 +6498,7 @@
         <v>6529</v>
       </c>
       <c r="C433">
-        <v>6.8938262462615967</v>
+        <v>4.5527992248535156</v>
       </c>
       <c r="D433">
         <v>1</v>
@@ -6512,7 +6512,7 @@
         <v>6207</v>
       </c>
       <c r="C434">
-        <v>6.997612476348877</v>
+        <v>4.7098629474639893</v>
       </c>
       <c r="D434">
         <v>1</v>
@@ -6526,7 +6526,7 @@
         <v>8991</v>
       </c>
       <c r="C435">
-        <v>13.607578754425051</v>
+        <v>8.6284792423248291</v>
       </c>
       <c r="D435">
         <v>1</v>
@@ -6540,7 +6540,7 @@
         <v>981</v>
       </c>
       <c r="C436">
-        <v>0.39059162139892578</v>
+        <v>0.26672697067260742</v>
       </c>
       <c r="D436">
         <v>1</v>
@@ -6554,7 +6554,7 @@
         <v>4736</v>
       </c>
       <c r="C437">
-        <v>4.8515183925628662</v>
+        <v>3.1226813793182369</v>
       </c>
       <c r="D437">
         <v>1</v>
@@ -6568,7 +6568,7 @@
         <v>5044</v>
       </c>
       <c r="C438">
-        <v>4.6096870899200439</v>
+        <v>3.3053028583526611</v>
       </c>
       <c r="D438">
         <v>1</v>
@@ -6582,7 +6582,7 @@
         <v>2514</v>
       </c>
       <c r="C439">
-        <v>1.922605037689209</v>
+        <v>1.2575733661651609</v>
       </c>
       <c r="D439">
         <v>1</v>
@@ -6596,7 +6596,7 @@
         <v>2494</v>
       </c>
       <c r="C440">
-        <v>1.8263509273529051</v>
+        <v>1.149695158004761</v>
       </c>
       <c r="D440">
         <v>1</v>
@@ -6610,7 +6610,7 @@
         <v>17782</v>
       </c>
       <c r="C441">
-        <v>42.676220655441277</v>
+        <v>28.37506628036499</v>
       </c>
       <c r="D441">
         <v>1</v>
@@ -6624,7 +6624,7 @@
         <v>434</v>
       </c>
       <c r="C442">
-        <v>0.22192096710205081</v>
+        <v>0.14317917823791501</v>
       </c>
       <c r="D442">
         <v>1</v>
@@ -6638,7 +6638,7 @@
         <v>7247</v>
       </c>
       <c r="C443">
-        <v>8.8941957950592041</v>
+        <v>7.52823805809021</v>
       </c>
       <c r="D443">
         <v>1</v>
@@ -6652,7 +6652,7 @@
         <v>1229</v>
       </c>
       <c r="C444">
-        <v>0.86612057685852051</v>
+        <v>0.61029720306396484</v>
       </c>
       <c r="D444">
         <v>1</v>
@@ -6666,7 +6666,7 @@
         <v>10791</v>
       </c>
       <c r="C445">
-        <v>15.52328944206238</v>
+        <v>10.39438796043396</v>
       </c>
       <c r="D445">
         <v>1</v>
@@ -6680,7 +6680,7 @@
         <v>5086</v>
       </c>
       <c r="C446">
-        <v>4.9709138870239258</v>
+        <v>3.4600479602813721</v>
       </c>
       <c r="D446">
         <v>1</v>
@@ -6694,7 +6694,7 @@
         <v>4479</v>
       </c>
       <c r="C447">
-        <v>4.3841350078582764</v>
+        <v>2.7561769485473628</v>
       </c>
       <c r="D447">
         <v>1</v>
@@ -6708,7 +6708,7 @@
         <v>13583</v>
       </c>
       <c r="C448">
-        <v>23.364272356033329</v>
+        <v>16.96275520324707</v>
       </c>
       <c r="D448">
         <v>1</v>
@@ -6722,7 +6722,7 @@
         <v>12504</v>
       </c>
       <c r="C449">
-        <v>20.447306632995609</v>
+        <v>15.736046075820919</v>
       </c>
       <c r="D449">
         <v>1</v>
@@ -6736,7 +6736,7 @@
         <v>816</v>
       </c>
       <c r="C450">
-        <v>0.46130919456481928</v>
+        <v>0.32931828498840332</v>
       </c>
       <c r="D450">
         <v>1</v>
@@ -6750,7 +6750,7 @@
         <v>1668</v>
       </c>
       <c r="C451">
-        <v>1.0373954772949221</v>
+        <v>0.82833290100097656</v>
       </c>
       <c r="D451">
         <v>1</v>
@@ -6764,7 +6764,7 @@
         <v>2729</v>
       </c>
       <c r="C452">
-        <v>1.951093196868896</v>
+        <v>1.395344018936157</v>
       </c>
       <c r="D452">
         <v>1</v>
@@ -6778,7 +6778,7 @@
         <v>10816</v>
       </c>
       <c r="C453">
-        <v>17.327660799026489</v>
+        <v>12.46210789680481</v>
       </c>
       <c r="D453">
         <v>1</v>
@@ -6792,7 +6792,7 @@
         <v>2049</v>
       </c>
       <c r="C454">
-        <v>1.6215236186981199</v>
+        <v>1.211089134216309</v>
       </c>
       <c r="D454">
         <v>1</v>
@@ -6806,7 +6806,7 @@
         <v>6526</v>
       </c>
       <c r="C455">
-        <v>6.9788320064544678</v>
+        <v>5.1469075679779053</v>
       </c>
       <c r="D455">
         <v>1</v>
@@ -6820,7 +6820,7 @@
         <v>10439</v>
       </c>
       <c r="C456">
-        <v>17.025979995727539</v>
+        <v>14.742508411407471</v>
       </c>
       <c r="D456">
         <v>1</v>
@@ -6834,7 +6834,7 @@
         <v>12344</v>
       </c>
       <c r="C457">
-        <v>20.803561210632321</v>
+        <v>15.48947548866272</v>
       </c>
       <c r="D457">
         <v>1</v>
@@ -6848,7 +6848,7 @@
         <v>9768</v>
       </c>
       <c r="C458">
-        <v>14.46340537071228</v>
+        <v>11.969018220901489</v>
       </c>
       <c r="D458">
         <v>1</v>
@@ -6862,7 +6862,7 @@
         <v>2324</v>
       </c>
       <c r="C459">
-        <v>1.7055075168609619</v>
+        <v>1.4319872856140139</v>
       </c>
       <c r="D459">
         <v>1</v>
@@ -6876,7 +6876,7 @@
         <v>6551</v>
       </c>
       <c r="C460">
-        <v>6.3581106662750244</v>
+        <v>4.8474876880645752</v>
       </c>
       <c r="D460">
         <v>1</v>
@@ -6890,7 +6890,7 @@
         <v>2811</v>
       </c>
       <c r="C461">
-        <v>1.993494033813477</v>
+        <v>1.417273998260498</v>
       </c>
       <c r="D461">
         <v>1</v>
@@ -6904,7 +6904,7 @@
         <v>5827</v>
       </c>
       <c r="C462">
-        <v>6.5236620903015137</v>
+        <v>4.5312130451202393</v>
       </c>
       <c r="D462">
         <v>1</v>
@@ -6918,7 +6918,7 @@
         <v>6892</v>
       </c>
       <c r="C463">
-        <v>7.9068934917449951</v>
+        <v>6.0768265724182129</v>
       </c>
       <c r="D463">
         <v>1</v>
@@ -6932,7 +6932,7 @@
         <v>4817</v>
       </c>
       <c r="C464">
-        <v>4.3074922561645508</v>
+        <v>3.51691722869873</v>
       </c>
       <c r="D464">
         <v>1</v>
@@ -6946,7 +6946,7 @@
         <v>3302</v>
       </c>
       <c r="C465">
-        <v>2.6075057983398442</v>
+        <v>2.0176153182983398</v>
       </c>
       <c r="D465">
         <v>1</v>
@@ -6960,7 +6960,7 @@
         <v>7495</v>
       </c>
       <c r="C466">
-        <v>7.8390772342681876</v>
+        <v>5.8377950191497803</v>
       </c>
       <c r="D466">
         <v>1</v>
@@ -6974,7 +6974,7 @@
         <v>11124</v>
       </c>
       <c r="C467">
-        <v>19.545102596282959</v>
+        <v>14.93817353248596</v>
       </c>
       <c r="D467">
         <v>1</v>
@@ -6988,7 +6988,7 @@
         <v>8861</v>
       </c>
       <c r="C468">
-        <v>11.309963703155519</v>
+        <v>8.1383817195892334</v>
       </c>
       <c r="D468">
         <v>1</v>
@@ -7002,7 +7002,7 @@
         <v>5687</v>
       </c>
       <c r="C469">
-        <v>5.7987792491912842</v>
+        <v>3.7181282043457031</v>
       </c>
       <c r="D469">
         <v>1</v>
@@ -7016,7 +7016,7 @@
         <v>7253</v>
       </c>
       <c r="C470">
-        <v>8.4619221687316895</v>
+        <v>6.3612895011901864</v>
       </c>
       <c r="D470">
         <v>1</v>
@@ -7030,7 +7030,7 @@
         <v>10042</v>
       </c>
       <c r="C471">
-        <v>13.050546646118161</v>
+        <v>10.73122453689575</v>
       </c>
       <c r="D471">
         <v>1</v>
@@ -7044,7 +7044,7 @@
         <v>969</v>
       </c>
       <c r="C472">
-        <v>0.61157107353210449</v>
+        <v>0.41358113288879389</v>
       </c>
       <c r="D472">
         <v>1</v>
@@ -7058,7 +7058,7 @@
         <v>1907</v>
       </c>
       <c r="C473">
-        <v>1.1992654800415039</v>
+        <v>0.81920361518859863</v>
       </c>
       <c r="D473">
         <v>1</v>
@@ -7072,7 +7072,7 @@
         <v>7147</v>
       </c>
       <c r="C474">
-        <v>8.0301487445831299</v>
+        <v>6.3525948524475098</v>
       </c>
       <c r="D474">
         <v>1</v>
@@ -7086,7 +7086,7 @@
         <v>8361</v>
       </c>
       <c r="C475">
-        <v>9.7900347709655762</v>
+        <v>8.2807202339172363</v>
       </c>
       <c r="D475">
         <v>1</v>
@@ -7100,7 +7100,7 @@
         <v>14313</v>
       </c>
       <c r="C476">
-        <v>22.792531967163089</v>
+        <v>19.111879825592041</v>
       </c>
       <c r="D476">
         <v>1</v>
@@ -7114,7 +7114,7 @@
         <v>14415</v>
       </c>
       <c r="C477">
-        <v>24.369122505187988</v>
+        <v>19.627471208572391</v>
       </c>
       <c r="D477">
         <v>1</v>
@@ -7128,7 +7128,7 @@
         <v>17818</v>
       </c>
       <c r="C478">
-        <v>36.709075927734382</v>
+        <v>33.171278476715088</v>
       </c>
       <c r="D478">
         <v>1</v>
@@ -7142,7 +7142,7 @@
         <v>6020</v>
       </c>
       <c r="C479">
-        <v>5.7237393856048584</v>
+        <v>4.3869922161102286</v>
       </c>
       <c r="D479">
         <v>1</v>
@@ -7156,7 +7156,7 @@
         <v>4193</v>
       </c>
       <c r="C480">
-        <v>3.401828289031982</v>
+        <v>2.6750597953796391</v>
       </c>
       <c r="D480">
         <v>1</v>
@@ -7170,7 +7170,7 @@
         <v>8301</v>
       </c>
       <c r="C481">
-        <v>9.617072582244873</v>
+        <v>7.5331981182098389</v>
       </c>
       <c r="D481">
         <v>1</v>
@@ -7184,7 +7184,7 @@
         <v>4576</v>
       </c>
       <c r="C482">
-        <v>3.411797046661377</v>
+        <v>2.953443288803101</v>
       </c>
       <c r="D482">
         <v>1</v>
@@ -7198,7 +7198,7 @@
         <v>996</v>
       </c>
       <c r="C483">
-        <v>0.41958999633789063</v>
+        <v>0.36855459213256841</v>
       </c>
       <c r="D483">
         <v>1</v>
@@ -7212,7 +7212,7 @@
         <v>11864</v>
       </c>
       <c r="C484">
-        <v>17.588043212890621</v>
+        <v>14.775147199630741</v>
       </c>
       <c r="D484">
         <v>1</v>
@@ -7226,7 +7226,7 @@
         <v>5530</v>
       </c>
       <c r="C485">
-        <v>4.5903875827789307</v>
+        <v>4.0335080623626709</v>
       </c>
       <c r="D485">
         <v>1</v>
@@ -7240,7 +7240,7 @@
         <v>10476</v>
       </c>
       <c r="C486">
-        <v>13.176538705825809</v>
+        <v>12.53589534759521</v>
       </c>
       <c r="D486">
         <v>1</v>
@@ -7254,7 +7254,7 @@
         <v>8423</v>
       </c>
       <c r="C487">
-        <v>7.8630468845367432</v>
+        <v>7.0743775367736816</v>
       </c>
       <c r="D487">
         <v>1</v>
@@ -7268,7 +7268,7 @@
         <v>6243</v>
       </c>
       <c r="C488">
-        <v>5.5730869770050049</v>
+        <v>5.1611301898956299</v>
       </c>
       <c r="D488">
         <v>1</v>
@@ -7282,7 +7282,7 @@
         <v>4878</v>
       </c>
       <c r="C489">
-        <v>3.876203060150146</v>
+        <v>3.1327838897705078</v>
       </c>
       <c r="D489">
         <v>1</v>
@@ -7296,7 +7296,7 @@
         <v>6616</v>
       </c>
       <c r="C490">
-        <v>5.9334661960601807</v>
+        <v>5.5678510665893546</v>
       </c>
       <c r="D490">
         <v>1</v>
@@ -7310,7 +7310,7 @@
         <v>16098</v>
       </c>
       <c r="C491">
-        <v>29.42610144615173</v>
+        <v>25.46987152099609</v>
       </c>
       <c r="D491">
         <v>1</v>
@@ -7324,7 +7324,7 @@
         <v>4822</v>
       </c>
       <c r="C492">
-        <v>3.4288589954376221</v>
+        <v>3.019051313400269</v>
       </c>
       <c r="D492">
         <v>1</v>
@@ -7338,7 +7338,7 @@
         <v>1233</v>
       </c>
       <c r="C493">
-        <v>0.54666614532470703</v>
+        <v>0.51426124572753906</v>
       </c>
       <c r="D493">
         <v>1</v>
@@ -7352,7 +7352,7 @@
         <v>7739</v>
       </c>
       <c r="C494">
-        <v>7.2152900695800781</v>
+        <v>6.655339241027832</v>
       </c>
       <c r="D494">
         <v>1</v>
@@ -7366,7 +7366,7 @@
         <v>4743</v>
       </c>
       <c r="C495">
-        <v>3.9249775409698491</v>
+        <v>3.030831098556519</v>
       </c>
       <c r="D495">
         <v>1</v>
@@ -7380,7 +7380,7 @@
         <v>19653</v>
       </c>
       <c r="C496">
-        <v>40.579349756240838</v>
+        <v>37.170368194580078</v>
       </c>
       <c r="D496">
         <v>1</v>
@@ -7394,7 +7394,7 @@
         <v>16449</v>
       </c>
       <c r="C497">
-        <v>23.881574630737301</v>
+        <v>24.479380130767819</v>
       </c>
       <c r="D497">
         <v>1</v>
@@ -7408,7 +7408,7 @@
         <v>4157</v>
       </c>
       <c r="C498">
-        <v>2.1637673377990718</v>
+        <v>2.3383841514587398</v>
       </c>
       <c r="D498">
         <v>1</v>
@@ -7422,7 +7422,7 @@
         <v>3742</v>
       </c>
       <c r="C499">
-        <v>2.2608282566070561</v>
+        <v>2.3506183624267578</v>
       </c>
       <c r="D499">
         <v>1</v>
@@ -7436,7 +7436,7 @@
         <v>2564</v>
       </c>
       <c r="C500">
-        <v>1.1857409477233889</v>
+        <v>1.209393978118896</v>
       </c>
       <c r="D500">
         <v>1</v>
@@ -7450,7 +7450,7 @@
         <v>8374</v>
       </c>
       <c r="C501">
-        <v>7.1943778991699219</v>
+        <v>7.7370316982269287</v>
       </c>
       <c r="D501">
         <v>1</v>

</xml_diff>